<commit_message>
update: adding api service agent and fixing bugs
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2478,6 +2478,3596 @@
         </is>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>NNQF8Z</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:17:23</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>401</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>AK0GXG</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:17:23</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>404</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>OP7AVB</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:17:50</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>200</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>39NP4Y</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:19:11</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>200</v>
+      </c>
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:hai
+###
+Answer:Salam Harmoni🙏
+Halo! Saya Shavira, Ganesha Virtual Assistant dari Universitas Pendidikan Ganesha. Ada yang bisa saya bantu?</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>YGO2PO</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:20:46</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>200</v>
+      </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam perjalanan akademik yang baru ini.</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HWMLWR</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:24:30</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>200</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudah ada akun google di hp.
+###
+Answer:[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>HD3NPV</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:34:41</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>200</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudah ada akun google di hp.
+###
+Answer:[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>63HD7P</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:35:55</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>200</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses mengenai akun SSO E-Ganesha atau Google Undiksha Anda terdapat anomali. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. 
+Atau Anda dapat mengecek pada kontak berikut untuk informasi lebih lanjut: [https://upttik.undiksha.ac.id/kontak-kami](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>9IUM72</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:36:30</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>200</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>IO2ENE</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:37:02</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>200</v>
+      </c>
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses mengenai akun SSO E-Ganesha atau Google Undiksha Anda terdapat anomali. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. 
+Atau Anda dapat mengecek pada kontak berikut untuk informasi lebih lanjut: [https://upttik.undiksha.ac.id/kontak-kami](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>HIJWKJ</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:41:41</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>200</v>
+      </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Terjadi kesalahan dalam mendapatkan informasi reset akun SSO. Silakan coba lagi nanti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>RBPBNR</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:45:57</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>200</v>
+      </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses mengenai akun SSO E-Ganesha atau Google Undiksha Anda terdapat anomali. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. 
+Atau Anda dapat mengecek pada kontak berikut untuk informasi lebih lanjut: [https://upttik.undiksha.ac.id/kontak-kami](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>9W4J5D</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:47:33</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>200</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Berita terbaru. Saya lupa password sso sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi terbaru dari Universitas Pendidikan Ganesha (Undiksha):
+1. **FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak**
+   - **Tanggal:** 20 November 2024
+   - **Deskripsi:** Pusat Kajian Gender dan Anak LPPM Undiksha menyelenggarakan Focus Group Discussion untuk mendukung kesadaran gender dan perlindungan anak.
+   - [Baca selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)
+2. **Undiksha Gelar Pelatihan Penyusunan Proposal PkM bagi Dosen Muda**
+   - **Tanggal:** 20 November 2024
+   - **Deskripsi:** Undiksha menggelar pelatihan penyusunan proposal Pengabdian kepada Masyarakat untuk dosen muda.
+   - [Baca selengkapnya](https://undiksha.ac.id/undiksha-gelar-pelatihan-penyusunan-proposal-pkm-bagi-dosen-muda/)
+3. **Gelar Pelatihan Penyusunan Proposal, Undiksha Dorong Dosen Lakukan Penelitian Berdampak**
+   - **Tanggal:** 19 November 2024
+   - **Deskripsi:** Pelatihan penyusunan proposal penelitian bagi dosen untuk mendorong penelitian yang berdampak.
+   - [Baca selengkapnya](https://undiksha.ac.id/gelar-pelatihan-penyusunan-proposal-undiksha-dorong-dosen-lakukan-penelitian-berdampak/)
+4. **Undiksha Jadi Tujuan “Benchmarking” Universitas PGRI Adi Buana**
+   - **Tanggal:** 18 November 2024
+   - **Deskripsi:** Universitas PGRI Adi Buana melakukan kunjungan benchmarking ke Undiksha.
+   - [Baca selengkapnya](https://undiksha.ac.id/undiksha-jadi-tujuan-benchmarking-universitas-pgri-adi-buana/)
+5. **Hasil Seleksi Kompetensi Dasar Seleksi Penerimaan Calon Pegawai Negeri Sipil (CPNS) Kementerian Pendidikan, Kebudayaan, Riset, Dan Teknologi Tahun Anggaran 2024**
+   - **Tanggal:** 18 November 2024
+   - **Deskripsi:** Pengumuman hasil seleksi kompetensi dasar CPNS Kemdikbudristek tahun anggaran 2024.
+   - [Baca selengkapnya](https://undiksha.ac.id/hasil-skd-cpns-kemdikbudristek-2024/)
+Untuk informasi mengenai akun SSO E-Ganesha atau Google Undiksha, jika terdapat anomali, silakan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. Anda juga dapat menghubungi melalui [tautan ini](https://upttik.undiksha.ac.id/kontak-kami) untuk informasi lebih lanjut.
+Selanjutnya, berikut adalah informasi kelulusan peserta SMBJM di Undiksha:
+- **Nomor Pendaftaran:** 3242000006
+- **Nama Siswa:** KADEK YUNI SEDANI
+- **Tanggal Lahir:** 30 November 2005
+- **Tahun Daftar:** 2024
+- **Pilihan Program Studi:** Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- **Status Kelulusan:** Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+Informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda adalah sebagai berikut:
+- **NIM:** 2115101014
+- **URL KTM:** [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=RzhucVZZYXNUVkZkdFoyR05lTkI4QlgxdkZ5TldtK2lhY0V4bXluRjJ1NHp3NG1tOVpxNzlLSmNCUlE4MUdNY3B3Z2xMeit0aHdlcGtIR0dPWXZBdTVUY0tiUjNTSXovZTZ0Smp4aXR6ZnhvV21EUFJhU0N0dHJoK204bWlJcFk1VjV3M1hSRGYzODFHWEF5RXNkai9yaFAxNEZQTFFxREhOL01Ib3IrNjF4Y0JGTkdOSnF3WEN1b25QRkNmeTZyREtVN0ZjUFdMVXg4UGpJRlZQanU4c2ZYTGQxRFBhZEdVSkFxY1lTczhwSnJWY1dpcFBqdnZVS3d5dm1yS005NURDMUFSMEFRTFVVdTJqZzd1MzNTaExPTjNubFJUMFRmWjgwWUhxTGFabU1qMGU5SzV1SmRBVUM2NnBrdTUwMEpGVU5WU0lCc1l3VTg2Ym9Bck1DSW50Tnc2cTZJM01VcXhFRXJSeEk0UTNqcktuTTZpUVhUVTdZWGFsNFRpWlBYL0xTZ1NNNFNpVHUxRDg3bE9ZaUZzc1Vpd2VWb01oK1RjQkZnK2lYMjBIUTR6dytJWlBkS3J0cjFxZFk9)
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>8T56J7</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:48:55</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>200</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya lupa password sso sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi yang dapat saya sampaikan:
+1. Terkait pengajuan proses akun SSO E-Ganesha atau Google Undiksha, terdapat anomali. Untuk memproses akun Anda, silakan datang langsung ke Kantor UPA TIK Undiksha. Anda juga dapat menghubungi melalui kontak yang tersedia di [sini](https://upttik.undiksha.ac.id/kontak-kami) untuk informasi lebih lanjut.
+2. Informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha:
+   - Nomor Pendaftaran: 3242000006
+   - Nama Siswa: KADEK YUNI SEDANI
+   - Tanggal Lahir: 30 November 2005
+   - Tahun Daftar: 2024
+   - Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - Status Kelulusan: Lulus
+   Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+3. Informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+   - NIM: 2115101014
+   - URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=cDlBQXV5bTZJSHFnSWVIc0NrMmcwS3A2Q2VxdWFHTFdISXFQcUhuM3JsdGlqWTNyYjBtUmkreUE2bEI4Y1E4M1BPeHRZM1kxQk5WZ1VNNkY5MXRyYXlyRmVrQlVIcjZobjlNcmRrdG1qT2RvcUM0M0k0aDJqMFZtSDlvUHJsYW8rNmx3YU1iNVozSU40NzBNNngzRUtiSVFMWVRySlU4Nk44WmpwdC9mUGRkQ2hlbkcvb2h0WjB4ZVRYMWZnRWV3eUEvOFpXV2FUZWZMWk8wbkZuUk9QM2RsQ2M0L3VTNmVwYTFwSTlnU3JIazlsWldTUW1JYVljOEFBakNEdHdmVk5pelZuYTJLc0NhSmF1WlJlajBLLzdETlBCSGl6OXBmckhYMU5UTkJRelhkYlhVOE9rQmNTUmZuU2IxRklpZ0FpSFhxS1lKTzZLcGFQYnJCWUFBRHg0bmNBelZaNjBnWGpEUm01MWJXdHVVYjdEUnVXdnN1YkdPcVNhdFNNWDI3bkdlTHpyVnkxb01rYmxDU1ovbXVkcU5GNzJtNXJodU5pM2V6MGF5bzBITTdwOXdFZ1BoVVdOMit4V2c9)
+4. Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>5O7TIM</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:49:49</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>200</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya lupa password sso sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi yang dapat saya sampaikan:
+1. Terkait pengajuan proses akun SSO E-Ganesha atau Google Undiksha, terdapat anomali. Untuk memproses akun Anda, silakan datang langsung ke Kantor UPA TIK Undiksha. Anda juga dapat menghubungi melalui kontak yang tersedia di [sini](https://upttik.undiksha.ac.id/kontak-kami) untuk informasi lebih lanjut.
+2. Informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha:
+   - Nomor Pendaftaran: 3242000006
+   - Nama Siswa: KADEK YUNI SEDANI
+   - Tanggal Lahir: 30 November 2005
+   - Tahun Daftar: 2024
+   - Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - Status Kelulusan: Lulus
+   Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+3. Informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+   - NIM: 2115101014
+   - URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=YTJYdlBUdWNFcVBnNnp6VEtETHY4Mk1XN3crbm1PVlVRWGw0Nlc3NzlRbDdyWnlqWDIrVzlNeFNIWlpGRnBwYWFCaTNQK0JvVmxDcnJpQ0xuUzdpbVFEdzFJTGNRWmtzM25qUmJOZ1FlN1ZzcHpvdmdhUEhpRW9YWFZqSlg2UHlXYno4cEpKWEVsWkJSTVNzNlQyRW9JREdSNVp4V1JQV0RSVjZLTE4yY0s0RWg1TWZRZ04wOWIwOTc5QTEwNjArT0REQlExeGd4eERZWFhZSHlHZi94NE9ibHVEakZ5VGFjQmtkeGluQ0YvVlprVkYxVWxNd3VjNkFxblNXNkI0eTFCYk1uYmRsQ1NiRWQwTlhyUUFOYm5oOElTV0dvWEVjNTRmSDhSZVdtRFNUa2VBam15MUV2TjdJOVZodkt2RGVmWVpmSkdUNmdiU3JMOGdTWGhsYWRvWmxhcVk0L2RFWkZKSUF1YllNZlhNeEx0U3U3N0IzVXpLQ3R5Z1pLNjRlSUowakFiUVkrb0xZOUNhSDVtcjF2Zk1rVWxXQzBieDI2Z1FuRVRsZ2FlWjBRdFhmUUxVWWduaFJZTW89).
+4. Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>U58SOX</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:50:44</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>200</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya lupa password sso sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi yang dapat saya sampaikan:
+1. Terkait pengajuan proses akun SSO E-Ganesha atau Google Undiksha, terdapat anomali. Untuk memproses akun Anda, silakan datang langsung ke Kantor UPA TIK Undiksha. Anda juga dapat menghubungi melalui kontak yang tersedia di [sini](https://upttik.undiksha.ac.id/kontak-kami) untuk informasi lebih lanjut.
+2. Informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha:
+   - Nomor Pendaftaran: 3242000006
+   - Nama Siswa: KADEK YUNI SEDANI
+   - Tanggal Lahir: 30 November 2005
+   - Tahun Daftar: 2024
+   - Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - Status Kelulusan: Lulus
+   Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+3. Informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+   - NIM: 2115101014
+   - URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=Yk1leTA4aldPbzdGRWlsZmNCMjFUVTJyNjVsdytLMWg3QUg1RVIxbHYzU09xYThmRC9kTkZWT1M0RXhyTGsxWFRmaTNPbGlaYmJJbXRBWmtUV2NZS2FDdlpMUHZ0dUJtNXhMbzZvZk92b3BFcHlUUVpRYi9mMGUzcmwwcG5qbXJTUjNQSW1CM2JlVWpwZFVMZHdldmtFWG0vdFlXb0tSY0srbUcyV1FrM0xrZVdNZkZUNWdzV1Y2SEwvSzRRNDkzVVV6Y04rNHpOdXgyb0krVDJjb1VLcktyR1RXVktZUGp1eWtSSXVPVGF5NWNUanJrTFZTRXRRcjhHbWlhWmJ4OXorei9TV0szMlVyQTdMTk5mQTBhd0hDV0VNSUpYWGFYQUxGQ2J2eDBFb0M2eDhiNUtTTTNNSklIdDdVNXlvL0hxbzFpR2JqVGxtcnFaWUZ6VkJwUkJmSlM3Z0dCZFBmanhHdlA3UitMZjdQU0xDbUJQK3ZNelZjMDJISERXcEEzZDkrRmIrMFh3bXkyS0dkUkxtS1NsSVQzL2RtbDdWUUtuenpYRW1saFZTME1EUmZGYW9lRUJFeURsb0U9)
+4. Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>PK40HI</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:51:14</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>200</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam perjalanan akademik Anda.
+Selain itu, berikut adalah informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=RnRBdUdOMjFzazhHTFBobHpXSEdON2dvd0xXdW1DUmhtVzUzZStFWng3UjM3aG05emkyWGU5S3d4V3RrckFGU2gvZ2FxWTl3OFFNLzY3d1F0dFkwR2lHU2ZocDE1WFFGNkpBcjRzd09kN1k0WjlsWm9ZYlBIUmh1N3U1cXJMYnRia1AzYldUVjVCaTFIZ0IyeUZEYU00RUJoRzFsbzRUVXE1TEd6NW5QU3lxeFRwRVhCZHIzV3lCL3pzTEFCMW41UGo0bXNLbjZVMGRKMWFsaGNFaFpDTURoTlFsa2Iyd2RuVDhWak1HNE1wYzIxNnJrNjVoekpZNm8zcXpGc0QzZUY5VVp2YmFNZ0dqQ2t5OXFVdG9tV0ZsaDdhWDhxeWo0WnBsbjk5NUdDR0tSZktlSjd5ZGt1K1VpZGdPejEyTkpDU3VGRzVGWXppckJUZk5hK1RrN2lyVlVXS0pSOFlnaXJYVm05Z1IvSU9PdXdZRVE5aWVnRm9zTEVnNlRvWHljT01EUnJ1U1ZBZ2dLYWREWmU5ZHFMKzFpMEVicXdWRzRKVzU3NWtvY1VRbVZDNG0wUGc0NXoxcHZPbEE9)
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>6S2KT2</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:51:40</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>200</v>
+      </c>
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha?
+###
+Answer:Salam Harmoni🙏
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>9A0ZAO</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:52:04</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>200</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha?
+###
+Answer:Salam Harmoni🙏
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>U99ON8</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:53:21</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>200</v>
+      </c>
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam perjalanan akademik Anda.
+Selain itu, berikut adalah informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=OG53Vm1GU1hQVlUyYjlsSU1wM0JLeXIwUFROQ1BYdlRQNU1Rektoa280TkIxTHZuMDRHQ0Ztc1dFb1VwU3p4TStYOUpCcmdsZDlPWnpIU2ZmdkZoWkk3OTl1ZXk4VUxzSCtqbVlLZE1wZkNIbjdtUzYvUXM3OVQ0bFlqRnZ0bUFObCtPQVUrVW9oUFdsTHFWb0lZWG5RWWVKeUdaVmllS1lPK1JlL29Lc29pNVlOWFgyU2gzcW9oc2hVS2FFbE9MUmMwNzBYaXVwV0lpWXlaVlBMWERVVDlnSHo0MmlRSWIyWnVEbG8wYWRoR0R2eDM2Q0ZETnNsMG84SlZvSWl3eWJjVm1LbytyUzNBNjdsNXc5cXdxekcyMHczQW5obVhmbTI2M1Vvbm9GUUJKUWpMcml5YTFYcllweittYmpGQUdURnI3NEo4ajVaa1BRSEl0YXEvVnh4dnIySHIvV0JaMDYzUGdDQTU3cG45ZkJ6c3NTRVNHSmxXMmU4Zy9QYXpENGt6MHU1Wm03UFVNQlREbjc5UXBEK1NZWWhFV2VSUVBMV0toRjdwdXlRMk9iV2RlRlZxc3ZVTURWNTA9)
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>A3534C</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:54:22</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>200</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam perjalanan akademik Anda.
+Selain itu, berikut adalah informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=UGlHZDYyTmdwRnBaS2NZYjdGeHFOME5XRXY3STQ0ZFczUkFzcitnZEFYb0tsdDI4cHVsSjhmZkdDTm90TVIzRVh5TlRMcmRKMXozcVBPaTNzVWZDa0dRRXZxU0E0YnhHS2x0NXdmakdxalVaa3plTDFPcjBzT2gyTHFKM0ZGMmhhOXZvcFBxbnd0TG8xQ0VPbS9rTU5lcVFteEZLMGlzSFFiWE4vMkVBZlRlQXA2RnhMeWM5WCsxNSswSXhDQWNJTkJja3FaaGVOL3Bqd1dPR0JEbVB6RjVPc28yVHQ4ZXlLZSt1SVdYdnZOY2dDRE1MRFBDWXZzOGo2RE4xaDhvUWRXNnNkTnRjWWlWaHkydVJIYXJ1SjZRLzhIdHIvanRxVmYzcFdhRTdKK2tBUVdBbk9UUm83VkJoaTdMNW8vRzNjVzcxMmE1QWUxUk9saWc0ZHdNK3Y3VEZwaHNmYnU0dUNWektaUWlOU3l4QnphSXFZL1V4QU9rSGd6L0hjVkhMaXgwT1NldE9NV1hYaGlycUp4MEVUTi93bWJnaG44eGJDMWdic2NoQVY4MFIxRWp3VVEvbHpxMzRoc0U9)
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>1QXIYH</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2024-11-20 19:55:37</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>200</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Terjadi kesalahan dalam mendapatkan informasi reset akun SSO. Silakan coba lagi nanti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>9JSFKZ</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:00:53</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>200</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Terjadi kesalahan dalam mendapatkan informasi reset akun SSO. Silakan coba lagi nanti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>4ZLQYX</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:02:05</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>200</v>
+      </c>
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam perjalanan akademik yang akan datang.</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>62RX84</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:06:06</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>200</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Terjadi kesalahan dalam mendapatkan informasi reset akun SSO. Silakan coba lagi nanti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>LKEDJS</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:11:09</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>200</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Terjadi kesalahan dalam mendapatkan informasi reset akun SSO. Silakan coba lagi nanti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>BW89NP</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:19:55</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>200</v>
+      </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Selamat, pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda berhasil! Berikut adalah informasi akun Anda:
+- Email Account User: gelgel.abdiutama@undiksha.ac.id
+- Tipe User: Tidak disebutkan
+- Status: Sudah Terkirim
+Petunjuk untuk Anda:
+1. Buka Aplikasi Gmail di HP atau melalui Browser pada Laptop/Desktop Anda.
+2. Pastikan Anda sudah masuk/login menggunakan akun Google dari Undiksha.
+3. Di Gmail, silahkan cek email Anda dari Undiksha.
+4. Silahkan tekan tombol reset password atau klik link reset passwordnya.
+5. Ikuti langkah untuk memasukkan password baru yang sesuai.
+6. Jika sudah berhasil, silahkan login kembali ke SSO E-Ganesha Undiksha.</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>5P0HTP</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:25:53</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>200</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Selamat, pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda berhasil! Berikut adalah informasi akun Anda:
+- Email Account User: gelgel.abdiutama@undiksha.ac.id
+- Tipe User: Mahasiswa
+- Status: Sudah Terkirim
+Petunjuk untuk Anda:
+1. Buka Aplikasi Gmail di HP atau melalui Browser pada Laptop/Desktop Anda.
+2. Pastikan Anda sudah masuk/login menggunakan akun Google dari Undiksha.
+3. Di Gmail, silahkan cek email Anda dari Undiksha.
+4. Silahkan tekan tombol reset password atau klik link reset passwordnya.
+5. Ikuti langkah untuk memasukkan password baru yang sesuai.
+6. Jika sudah berhasil, silahkan login kembali ke SSO E-Ganesha Undiksha.
+Jika ada pertanyaan lebih lanjut, jangan ragu untuk bertanya!</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>E1IXUS</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:27:30</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>200</v>
+      </c>
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Terjadi kesalahan dalam mendapatkan informasi reset akun SSO. Silakan coba lagi nanti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>LYX62X</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:28:01</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>200</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Informasi yang diberikan adalah: "Silakan coba lagi nanti."</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>RW0NAQ</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:29:34</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>200</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Terjadi kesalahan dalam mendapatkan informasi reset akun SSO. Silakan coba lagi nanti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>BHFU5C</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:32:13</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>200</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Selamat, pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda berhasil! Berikut adalah informasi akun Anda:
+- Email Account User: gelgel.abdiutama@undiksha.ac.id
+- Tipe User: Mahasiswa
+- Status: Sudah Terkirim
+Petunjuk untuk Anda:
+1. Buka Aplikasi Gmail di HP atau melalui Browser pada Laptop/Desktop Anda.
+2. Pastikan Anda sudah masuk/login menggunakan akun Google dari Undiksha.
+3. Di Gmail, silahkan cek email Anda dari Undiksha.
+4. Silahkan tekan tombol reset password atau klik link reset passwordnya.
+5. Ikuti langkah untuk memasukkan password baru yang sesuai.
+6. Jika sudah berhasil, silahkan login kembali ke SSO E-Ganesha Undiksha.
+Jika ada pertanyaan lebih lanjut, jangan ragu untuk bertanya!</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>4D80O5</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:32:25</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>200</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Berikut adalah informasi mengenai kesalahannya:
+- Info: Anda telah melakukan reset password, silahkan cek email dan coba lagi nanti.
+Jika Anda masih mengalami kesulitan, silakan hubungi layanan bantuan untuk mendapatkan bantuan lebih lanjut.</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>PYI8UQ</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:35:36</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>200</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Berikut adalah informasi mengenai kesalahannya:
+- Anda telah melakukan reset password sebelumnya, silahkan cek email Anda dan coba lagi nanti.
+Jika Anda memerlukan bantuan lebih lanjut, jangan ragu untuk menghubungi layanan dukungan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>TXIQNH</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:36:13</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>200</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Anda telah melakukan reset password sebelumnya, jadi silahkan cek email Anda dan coba lagi nanti. Jika ada pertanyaan lebih lanjut, jangan ragu untuk menghubungi layanan bantuan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>TZRXDZ</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:38:13</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>200</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:cetak ktm 1010101010
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 1010101010
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/1010101010?token=TXo2V1lvbnRmNDdJQXBRWVN0RVlxY2d3V2UxVFpJYm5VUTA4VXpKb3c1bU5XTFJKR1RvTTNJdC9XR29Sc25OSE5lS1phR2VDeGtpWHdKTWp0LzhFdW1wMmxJT2FuQmUxQVlnVkxScGVsb0tkRnpWR2NtNFR1amtGNUMyWUE0Vm10djRyWjlmWXplN2szVEJ2UWpvTFFmYTQyZ0NlUFVUc1F4WU83N2ZkZG13MXVEK2FMNkd5WEJXdTFPR1ltV2p3cXRVc2g3RnRKODF1b0xZWDFRaVhSUDJwdXc4cXNjLzZNdzN1WU1rbWZGV1BsSjJCbTB5L0w2d1E1UVNsWXFka0NCUkR1YXE4N2tHTElXMC9yZ3BGaTF0K3RxcjFyNno2YWRNRkE2TXJOVHNVbm9GdTYyTWVRSVpyd05rdWdVcFA2QWdKRzVlM1hUV2tGMnZ4a3gvYlFoMnJlR3cyT04vVjVrZXFqdTRzQkJPSEpHeEZoVmJ6eUJhWFZQMUJYOGZuQTUxZmdnRVZ0Vm4rV25wcFA5WGsrQmdQbUNxUmlwS3JaVkJHK1BWdFF6TjZkbFhtMEozSVJZd1g5ZWc9).
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>BDYW3P</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:38:54</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>200</v>
+      </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:cetak ktm 2115101014
+###
+Answer:Salam Harmoni🙏
+Berikut informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=NTdHMmFyUlJKWHdqcUZ0dHdadGJzT2dOR2tmOFJ0NEhNSWVuNnRJb2VnbWs4Mk53aVhtMHR3YWErRkRUeC80Q25TTXM1dlpla3JFRHhQekE4UnpOZHBOdXRGR0I4SFF1MnhGbUV6bVcxTzA0MHdpeE8rbGV4Q2FROWJvM3Y4ejJxamxQVWZNQXIrZndzSnoyY2pvcTZ0WnNVUWlpV2p3dXZsNVYxMUZzS0p5YVVHY2hPSExVZi94b3FyaXVpK2xkcWhZNEJ0cU9XeGZwZ3pTWnd0dHJUSHpzWW1TTTBTNGZ4T1pySDIyM1B0VDNrMzdaYjlrUForN3BmMFVmZTVHSlJMK1dZbVN3Q3p3Zkk1Z1JVYlkxZEdDMTArUFQzSVdoNHBwb2w5anpSSDVHRkF6VGh0WGc4dkRCUlIzZ2lQZGVReEhoOStCdkdia096VC9HNFNKcDRQWDNoZ0ZRTWNKYk9Jbm4xSUZiazNWZUdSSGtHYjVKNU51cFlpaWtrYTkyam5QWWRiZ2JVZEtFdHJtUjJLVU9sdXA5Rm1xcW9NSnVmZnhDRldUMjl0bXkwY2VFY2NuS1g2b2RzNEk9)
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>233B65</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:40:21</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>200</v>
+      </c>
+      <c r="E105" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:cetak ktm 2115101014
+###
+Answer:Salam Harmoni🙏
+Berikut informasi Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=bWVMQ280RjdwNjMwcHdIWG1RbTdEeDZIOFBObXBzaTJyUDhkaTl2OHplRjFQZFNRVUgvRlBPT2RoUmtQWE9xQk95bSsxRnVxcmorVW1LQjN4SkI5Zkh6QzhqejNmSU1yRjBJb1FyVSt6dkxzemcvZWpsS0Uxc1RYcHFwNnN4dE84UVNmTk1xRXd3YjBKcWtBSFNmcU5ibk5ZNXowbEpndXMvVWZVZkppaXZvVy9sbjU0K0w3QzdYanVWNVJtSEdVMStkL1FPVXZOSFEvb0dzNzJYQ25OQ0l3ZlJGQ2ZXOWlLZS9SWDZwV3ppNjNVUnI0MHlLcVArakljdE9yWlp4enlEYzR6QnB4cVF1b2dyY3N3WUozRkU0ODVWRWtyTHBEN29odEh3blg2K3RVLzhJTmhEd0pxamxERzhYZ1lRdjRFclVCZjhYM2trNmRWVGN5NTBvdGJQc0ZsOGJLNk1vekp2ZjdwV1RyaGtiRjljUjJTL2o4VUxjRmdaMjRzU3U5VnA0TGRyL3JmZitjSmZiek9WYk1OQW9aRC91R01BVjRmREhyRXpiQ1p1akZ1WHRGZU5NeTNNT042ZFE9)
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>35Z3RH</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:44:13</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>200</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:cetak ktm 2115101014
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=eTI1YmVodG50Qmhub2dndkpTT2xGeDhEVTJTb0wraWtZbDFSSklidTdJTThBTTFJa0lzeWx2UkQxL1AzclNtSWIvM0pHNDd2QStoT2kwbGRXcmZBU2hIcW54NHFxQ3JMSFJKWG5nQ25PMWhCeTBxMkc5aGhEVmFwSFhaWGNVcGZuNnZHZTRZSmx6YW5hMnF6NnlWMTNTRU4yOVBscURzOGF6UHFCRldBYUY3YjNuMFZ3TWhiS01LbE0rTGd2bHNFbFFVS2lRZEViSzNBbmYwalJEQnVBamVZdll0WjhMdDh4YU5ibzRQODBYNkZXZ09pdmZLeFBCMndqQkZITEZaeHNKSUY1cDNlT1BFSGRSODJmMGVvTXNnUWFjMDA4K3UzZy9YU2FWT25HMUMrN0NqRzNHSWtFUFBodDlRZWt4U2Yra2hUd0JWMnlmc2ZSWDZlRXB4L3VHK3ozNjVnbndRVlBac0w2VTJ1eWc3RmlmM0UxME9XY1NBYWIwUTFzcEJZMEdpaEVweU11cTFmR1R5YzNjREEwQlliNkNQZGpEZHBWbWdON2hhSWxXQ1F6VUtXOGx6NDl2SmxTT1k9).
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>OEQKJQ</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:44:25</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>200</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam perjalanan studi Anda.</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>83UOEW</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:47:53</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>200</v>
+      </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung dan menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam menjalani studi dan mencapai cita-cita.</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>VY2OWC</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:48:44</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>200</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses mengenai akun SSO E-Ganesha atau Google Undiksha Anda terdapat anomali. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. 
+Atau Anda dapat mengecek pada kontak berikut untuk informasi lebih lanjut: [https://upttik.undiksha.ac.id/kontak-kami](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>JLJU1Z</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:49:02</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>200</v>
+      </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Selamat, pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda berhasil! Berikut adalah informasi akun Anda:
+- Email Account User: gelgel.abdiutama@undiksha.ac.id
+- Tipe User: Mahasiswa
+- Status: Sudah Terkirim
+Petunjuk untuk Anda:
+1. Buka Aplikasi Gmail di HP atau melalui browser pada laptop/desktop Anda.
+2. Pastikan Anda sudah masuk/login menggunakan akun Google dari Undiksha.
+3. Di Gmail, silahkan cek email Anda dari Undiksha.
+4. Silahkan tekan tombol reset password atau klik link reset passwordnya.
+5. Ikuti langkah untuk memasukkan password baru yang sesuai.
+6. Jika sudah berhasil, silahkan login kembali ke SSO E-Ganesha Undiksha.
+Jika ada pertanyaan lebih lanjut, jangan ragu untuk bertanya!</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>XZVS10</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:50:09</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>200</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Anda telah melakukan reset password sebelumnya, jadi silahkan cek email Anda dan coba lagi nanti. Jika ada pertanyaan lebih lanjut, jangan ragu untuk menghubungi layanan bantuan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2XFQG4</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:50:53</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>200</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Anda telah melakukan reset password sebelumnya, jadi silahkan cek email Anda dan coba lagi nanti. Jika ada pertanyaan lebih lanjut, jangan ragu untuk menghubungi layanan bantuan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>YFD5AS</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:51:47</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>200</v>
+      </c>
+      <c r="E113" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil! Anda telah melakukan reset password sebelumnya, silahkan cek email Anda dan coba lagi nanti. Jika Anda masih mengalami kesulitan, Anda dapat menghubungi pihak IT Undiksha untuk bantuan lebih lanjut.</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>C5172V</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:53:05</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>200</v>
+      </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Anda telah melakukan reset password sebelumnya, jadi silahkan cek email Anda dan coba lagi nanti. Jika ada pertanyaan lebih lanjut, jangan ragu untuk menghubungi layanan bantuan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>N8F5JX</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:54:15</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>200</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:berikan 1 berita saja
+###
+Answer:Salam Harmoni🙏
+Berita terbaru yang dapat saya sampaikan adalah:
+**Judul:** FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak  
+**Tanggal Publikasi:** Rabu, 20 November 2024  
+**Deskripsi:** Singaraja - Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Universitas Pendidikan Ganesha (Undiksha) menyelenggarakan Focus Group.  
+**Link:** [Baca Selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>9IQ3QU</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:56:37</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>200</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Berikan 1 berita saja. Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi terbaru yang dapat saya sampaikan:
+1. **Berita Terbaru:**
+   - **Judul:** FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak
+   - **Tanggal Publikasi:** Rabu, 20 November 2024
+   - **Deskripsi:** Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Universitas Pendidikan Ganesha (Undiksha) telah menyelenggarakan Focus Group.
+   - **Link:** [Baca Selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)
+2. **Informasi Akun SSO E-Ganesha:**
+   - Selamat, pengajuan proses reset password akun SSO E-Ganesha Undiksha berhasil!
+   - **Email Account User:** gelgel.abdiutama@undiksha.ac.id
+   - **Tipe User:** Mahasiswa
+   - **Status:** Sudah Terkirim
+   - **Petunjuk:** Silakan buka aplikasi Gmail dan cek email dari Undiksha untuk melakukan reset password.
+3. **Kelulusan Peserta SMBJM di Undiksha:**
+   - **Nomor Pendaftaran:** 3242000006
+   - **Nama Siswa:** KADEK YUNI SEDANI
+   - **Tanggal Lahir:** 30 November 2005
+   - **Tahun Daftar:** 2024
+   - **Pilihan Program Studi:** Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - **Status Kelulusan:** Lulus
+   - Ucapan selamat bergabung di Universitas Pendidikan Ganesha untuk KADEK YUNI SEDANI.
+4. **Informasi Kartu Tanda Mahasiswa (KTM):**
+   - **NIM:** 2115101014
+   - **URL KTM:** [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=elZPdVNVdDRvbU9RN09RNEk3cjJWdy9rdEh2L1Rud1RwU1ZQNnhoaUJsakwvcHp0SE8wQnRGeFN0RE5WTzhhVDZ1SGJtVG1DYVFVYllTdmhNRUFrR1lsc3c0NnRQdjBZZmdlSHg4bzZTcGdVZ0dvazEvTldLS0svd1dSZGYvMzZvNHI5TElyTDhjSFYxUGh2QVQrZGxrUEQ0QTdYTEZLclVQTmdFdzBxNjBmQ2w1Mm5XVEt6NXZiY1h3RDJSbUxkTVJ3YjByaktWTGxwOS96S085TGIwa0pGRjFUVDdtR0kzd0ZhYXJNRDNOVEgvTjJtb044VDZaUGFTdi9MWDJsODFOMlpKTDRVallmS1JGaFd1UFhMZ3ZZSWRMZWpXQkplQXY5emZodUZaVTVGaTFuaWU2c1NEamwwWk82QUlPYnBldEQzcGcyTlZKVk50VXNFNVppMTRWM2lZMlR6TFk2QVRaRXkwVDR5LzFKRVlUc0VQSVpCSWRQNENBS0IvK2JidnRvV0d4a0k3cGFPSTRxS29NeVB1WFRYaloyUmlmU3ByT1FlMWdMbE5oQkJpa1JXczJneUJORm5JODg9)
+5. **Rektor Universitas Pendidikan Ganesha:**
+   - Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>CPJP0M</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:58:13</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>200</v>
+      </c>
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudiartika@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Anda telah melakukan reset password sebelumnya, jadi silahkan cek email Anda dan coba lagi nanti. Jika ada pertanyaan lebih lanjut, jangan ragu untuk menghubungi layanan bantuan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>50M470</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:58:37</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>200</v>
+      </c>
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudiartika@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Anda telah melakukan reset password sebelumnya, jadi silahkan cek email Anda dan coba lagi nanti. Jika ada pertanyaan lebih lanjut, jangan ragu untuk menghubungi layanan bantuan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>5SU91T</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>2024-11-20 20:59:30</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>200</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudiartika@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. 
+Detail kesalahan yang diterima adalah: {"status":0,"message":"This email is not allowed"}.
+Silakan periksa kembali alamat email yang Anda gunakan atau hubungi pihak administrasi untuk bantuan lebih lanjut.</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>1P3PB9</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:00:59</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>200</v>
+      </c>
+      <c r="E120" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudiartika@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Kami mohon maaf, tetapi pengajuan proses reset password untuk akun SSO E-Ganesha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa alamat email yang Anda gunakan tidak diizinkan. 
+Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>HMO1Z8</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:02:17</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>200</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudiartika@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Kami mohon maaf, tetapi pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa alamat email yang Anda gunakan tidak diizinkan untuk melakukan reset password. 
+Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih.</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>DIJXN1</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:02:39</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>200</v>
+      </c>
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudiartika@asdasd sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses mengenai akun SSO E-Ganesha atau Google Undiksha Anda terdapat anomali. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. 
+Atau Anda dapat mengecek pada kontak berikut untuk informasi lebih lanjut: [https://upttik.undiksha.ac.id/kontak-kami](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>097EQR</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:02:53</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>200</v>
+      </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso afasdfadsf@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Kami informasikan bahwa pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima adalah "Email ini tidak diizinkan." 
+Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>3XJB96</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:03:15</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>200</v>
+      </c>
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso sudiartika@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Kami mohon maaf, tetapi pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa alamat email yang Anda gunakan tidak diizinkan untuk melakukan reset password.
+Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>71IOMR</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:03:36</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>200</v>
+      </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Selamat, pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda berhasil! Berikut adalah informasi akun Anda:
+- Email Account User: gelgel.abdiutama@undiksha.ac.id
+- Tipe User: Mahasiswa
+- Status: Sudah Terkirim
+Petunjuk untuk Anda:
+1. Buka Aplikasi Gmail di HP atau melalui Browser pada Laptop/Desktop Anda.
+2. Pastikan Anda sudah masuk/login menggunakan akun Google dari Undiksha.
+3. Di Gmail, silahkan cek email Anda dari Undiksha.
+4. Silahkan tekan tombol reset password atau klik link reset passwordnya.
+5. Ikuti langkah untuk memasukkan password baru yang sesuai.
+6. Jika sudah berhasil, silahkan login kembali ke SSO E-Ganesha Undiksha.
+Jika ada pertanyaan lebih lanjut, jangan ragu untuk bertanya!</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>VYVRBM</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:03:49</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>200</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso gelgel.abdiutama@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Kami informasikan bahwa pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa batas pengajuan reset password telah terlampaui. 
+Silakan coba lagi setelah beberapa waktu atau hubungi pihak administrasi untuk mendapatkan bantuan lebih lanjut. Terima kasih.</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>10IRFE</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:06:21</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>200</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Berikan 1 berita saja. Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi terbaru yang dapat saya sampaikan:
+1. **Berita Terbaru:**
+   - **Judul:** FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak
+   - **Tanggal Publikasi:** Rabu, 20 November 2024
+   - **Deskripsi:** Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Universitas Pendidikan Ganesha (Undiksha) telah menyelenggarakan Focus Group.
+   - **Link:** [Baca Selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)
+2. **Informasi Reset Password:**
+   - Pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan menunjukkan bahwa email yang digunakan tidak diizinkan untuk melakukan reset password. Silakan periksa kembali alamat email yang dimasukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut.
+3. **Kelulusan Peserta SMBJM:**
+   - **Nomor Pendaftaran:** 3242000006
+   - **Nama Siswa:** KADEK YUNI SEDANI
+   - **Tanggal Lahir:** 30 November 2005
+   - **Tahun Daftar:** 2024
+   - **Pilihan Program Studi:** Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - **Status Kelulusan:** Lulus
+   - Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+4. **Informasi Kartu Tanda Mahasiswa (KTM):**
+   - **NIM:** 2115101014
+   - **URL KTM:** [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=RlRRMXdNZlUwemZRQ0dXVmxTK295dnpzOFlKeis1ckZCY3ovRDE3YnNOVGxtUHRHbUJGanNKUmtBVVNlVjY5T2hLVDBydUNYb1duNWhUTjZZUEUvenBoZFlSSkdXK3MxR0IwV2haNXNEZXpzcmViSFkvQ0RKOGVsVWhZK0NXMHAyZ0NsVkpRWUFBQWZ1YzF5blhLdzV1bVBzUm5HZm5idE9wUFp1eFhnUHluVy9vMzdqcHZGWVJSVUI3c3VaOWJLVi9IQm82VEVjV3lpVndQb0ppQ3p3aFNuNy9BbjZoZHViK0JRZmVRaHltcWlxcWROQUU3VENiQjRQVWpZc1dESmZhT1BiNnZ0eGZydFhFYWVaL0JoV3NwVkNiK3dVVHlDR1lDaEU1dU9GcVpESm1PS2MyVnFQRVNtN0hHaEdWZ0ZESWlHVVNOZ0d4Rk5HcXJPWnFWdWwyWExKQTBPWnhIbEFSb0Z5RmM0eVBNTm5zendIanRXOWVyK0FSaUJSYno0Q3VBSXpDaUI5b3JGSk45cXE2VVY5bktxOEJFZFVVdjQ3OVVuZnovZVhzVVVjN0dsVEFDUlZVTzVwVmM9)
+5. **Rektor Universitas Pendidikan Ganesha:**
+   - Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd. 
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>0GA0Q3</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:08:41</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>200</v>
+      </c>
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Berikan 1 berita saja. Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp. Cetak ktm 2115101014.
+###
+Answer:Salam Harmoni🙏
+Berita terbaru yang dapat saya sampaikan adalah mengenai kegiatan yang diselenggarakan oleh Universitas Pendidikan Ganesha (Undiksha). Pada tanggal 20 November 2024, Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Undiksha mengadakan Focus Group Discussion (FGD) dengan Pemerintah Kabupaten Buleleng. Kegiatan ini bertujuan untuk mendukung peningkatan kesadaran gender dan perlindungan anak. Untuk informasi lebih lanjut, Anda dapat mengunjungi [link ini](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/).
+Selain itu, kami informasikan bahwa pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima adalah "Email ini tidak diizinkan." Silakan periksa kembali alamat email yang Anda gunakan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut.
+Berikut juga informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=T0tBcHh2cXgyOHNQMVpMTkxPWlpyaDVabExvZ0o3QkE2dVZaNFgvWnNnNXBPTGxpcmVnM0daeU1jbWVvd0xGUEh5aGtUMzcwazlvWi9xUWZlLzBVN0Z0MW1Lb1FMcFBscVNuOGMvb2VxTTIrQ29WRS80SVVTemNFTGIzckt4RGJUUFBVTno0VFBzTEVOZ0dxUjQ5WXJMNnZhU0V1bU1EVTlDemNDdUxSK3ZGQmNIQjluRnBsazdNUHQxWmlKVlQrVGQwd2ZyRFk5aWxBaTM3cXlwamJySEMrNTNjVlNKU0lGVHlDRm8ra0kzbUlyTkpFWDBtbE45WkhQcGx2WTVZaU95VmdYTkhDaHdTQzFuV1FpSHA3aW9BTldyeXU3RDh3eG10WktvcCtJa2RlT0d2V1NHdVl1OGwzTDJDMWVUMVZiUnFsVHdZdlNtUjAxYU84TWZRZ0YxNmhGbTBUbVcrUFJOU3o3R1U0WERFNU9sQzNabUd5TEFDWlFOaWNqeTExUVVKQnBqWUkySW0wQkRIWVMyZkFPYzhsamxySUxodk5PdHUxd2kybDhDc2F2MkFLZmhzMUlKOUVsVTA9).
+Terakhir, Rektor Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>FRMBCJ</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:09:31</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>200</v>
+      </c>
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Berikan 1 berita saja. Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Berita terbaru yang dapat saya sampaikan adalah sebagai berikut:
+**Judul:** FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak  
+**Tanggal Publikasi:** Rabu, 20 November 2024  
+**Deskripsi:** Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Universitas Pendidikan Ganesha (Undiksha) telah menyelenggarakan Focus Group Discussion (FGD) untuk mendukung peningkatan kesadaran gender dan perlindungan anak.  
+**Link:** [Baca Selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)
+Selain itu, kami mohon maaf bahwa pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa email yang Anda gunakan tidak diizinkan untuk melakukan reset password. Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!
+Rektor Universitas Pendidikan Ganesha (Undiksha) saat ini adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>FIS30F</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:10:28</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>200</v>
+      </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Berikan 1 berita saja.
+###
+Answer:Salam Harmoni🙏
+Berita terbaru yang dapat saya sampaikan adalah:
+**Judul:** FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak  
+**Tanggal Publikasi:** Wed, 20 Nov 2024  
+**Deskripsi:** Singaraja- Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Universitas Pendidikan Ganesha (Undiksha) menyelenggarakan Focus Group.  
+**Link:** [Baca Selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)
+Selain itu, Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>J3B0MM</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:10:41</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>200</v>
+      </c>
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha?
+###
+Answer:Salam Harmoni🙏
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>3BFESJ</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:11:10</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>200</v>
+      </c>
+      <c r="E132" t="b">
+        <v>1</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp.
+###
+Answer:Salam Harmoni🙏
+Kami informasikan bahwa pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima adalah "Email ini tidak diizinkan." Silakan periksa kembali alamat email yang Anda gunakan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!
+Selain itu, Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>C6GDGV</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:11:47</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>200</v>
+      </c>
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya lupa password sso email@undiksha.ac.id
+###
+Answer:Salam Harmoni🙏
+Kami mohon maaf, tetapi pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa email yang Anda gunakan tidak diizinkan untuk melakukan reset password. Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!
+Selain itu, Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>IK6OAK</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:12:24</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>200</v>
+      </c>
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya ingin reset password Google.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses mengenai akun SSO E-Ganesha atau Google Undiksha Anda terdapat anomali. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. Anda juga dapat mengecek informasi lebih lanjut melalui kontak yang tersedia di [sini](https://upttik.undiksha.ac.id/kontak-kami).
+Selain itu, Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>HUICA3</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:13:08</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>200</v>
+      </c>
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cetak ktm 2115101014.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=Wk4xUHlRY2RTVmd1ajVsZ25VNndmTkVQSWw3eWRWMzJOWk9SaHhReWZCMWtHK09oOFp3RW0yVjZ3YW16WXdjMER4OUxsY3hsdDdPMTJLZmphM3dlV3VQazFFZkhXUWFKWFU5cXBYcFp5MTc2MDl2aDcvdHZoa3ZPa1VzSGFtdGlaMXdOd0wxRVJHVXBoZTZScHFoL1l1cVVrZFdUNFNvSEJDQ1QybDJmNkVvUUdUMjhoQXRJSnlBbm05ZHdQc2JxNnR0K1dwMURWWlV1dUw0ZGsyYnQxSGFjUXgwVHduMkxYSHZWVUMzUGxEQkU5NzIzTzd4TzU5SGJlZVZZUTdYTmM5QTVTaUdyT1dTaWpWQkM3ckhkRm95Y1g1YmpEcXRwd0NPajg1WkpORExYbWRERWEzRG1Kb0JvbG1XUW54THVYVnZML05vclRKVEZlVkx4MFFOUThJaWVvSXRHcnZVMUhhN1hTaFZubER4bGMrNDF6bmUvNm9sVnNEOHNtWGxEL2ZqVFkzMTJ1SWNRMkZwVng1TXI5RUdNaE4wbmVPdmxCemJXWFFhcVkxc0xwS3FvUm43L1l6OGRVN2M9)
+Selain itu, Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>UN1M8L</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:13:26</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>200</v>
+      </c>
+      <c r="E136" t="b">
+        <v>1</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cetak ktm.
+###
+Answer:Salam Harmoni🙏
+Dari informasi yang ada, belum terdapat nomor NIM (Nomor Induk Mahasiswa) yang diberikan. NIM (Nomor Induk Mahasiswa) yang valid dari Undiksha berjumlah 10 digit angka. Format penulisan pesan yang harus diikuti adalah sebagai berikut:
+- KTM [NIM]
+Contoh penulisan pesan yang benar adalah:
+- KTM XXXXXXXXXX
+Kirimkan NIM yang benar pada pesan ini sesuai format dan contoh, agar bisa mencetak Kartu Tanda Mahasiswa (KTM).
+Selain itu, Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>JY5MC0</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:13:50</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>200</v>
+      </c>
+      <c r="E137" t="b">
+        <v>1</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam menjalani studi dan mencapai cita-cita. 
+Rektor Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2YBDUN</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:15:00</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>200</v>
+      </c>
+      <c r="E138" t="b">
+        <v>1</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha (Undiksha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam menjalani studi di program yang telah dipilih. 
+Rektor Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>01GXSK</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:15:30</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>200</v>
+      </c>
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Cek kelulusan
+###
+Answer:Salam Harmoni🙏
+Dari informasi yang ada, belum terdapat Nomor Pendaftaran dan Tanggal Lahir Pendaftar SMBJM yang diberikan. Untuk melakukan pengecekan kelulusan, Anda perlu mengikuti format penulisan pesan sebagai berikut:
+Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
+Sebagai contoh, penulisan pesan yang benar adalah:
+Cek Kelulusan Nomor Pendaftaran 3201928428 Tanggal Lahir 2005-01-30
+Pastikan untuk mengirimkan pesan sesuai format dan contoh yang telah diberikan agar dapat mengecek kelulusan SMBJM Undiksha.
+Selain itu, Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>FLI1TE</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:16:25</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>200</v>
+      </c>
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp. Cetak ktm 2115101014.
+###
+Answer:Salam Harmoni🙏
+Kami mohon maaf, tetapi pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa email yang Anda gunakan tidak diizinkan untuk melakukan reset password. 
+Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!
+Berikut informasi Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=anNyT25QYjM5ZkxpcmpCcjRoQnZpeVN1dHI4cTBwRmJ4TzlMZ3RUWmJ4MG14NTNDSjhuYkJhQTYrS0gzakwyTVR2Vmt5bnJ0RjhLeFY2TE5yeEhLVllDM05FL3ZSZXhBQXVyaFozWFlubEhRbkJEMzlGL0JYay9UdXNGZXpzT1JQZ3FMVFl6bFFTZ0dXZ3lQUVgrOVZBSm1lSlVJWWdkMFRuMHhUTFNidlBGWmhaZmZKTG94MkMwcFpjTkpIQ1FGNU04WEZHUmEreEZON0IyWEF4RE9Xc1RpYUdCazJUNHUyL0ZTVkFQV01NeVEzQUlOd3M2QjBTSFRpSUd3TnVVTmFQdnZ3Ukd2Vjh4S3ZJTzNqQ3kya0JSOGVWM0V3SlZaWnp5Y1A5TXQvRVoydGFiN3ovb2pDK0J2eWlZSFI5YTdSTzlyUkJBSXcvU2VOalZ0RFQyd2pvbVRlcnBaeEpYY0JIZ0MwL1ZTUDcweFoyaDhZT1lSUG42SDJPa293RkdncHFsek9LYkZaMWcvTWlTQ0YyM2IvTkl2K25QVTRhREJyTzdYQzVyVkkwdjBHOUxxMUY5V2RlV2xJR1E9)</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>76PHLQ</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:17:01</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>200</v>
+      </c>
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Kami mohon maaf, tetapi pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa alamat email yang Anda gunakan tidak diizinkan untuk melakukan reset password. Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!
+Berikut informasi Kelulusan Peserta SMBJM di Undiksha (Universitas Pendidikan Ganesha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 2005-11-30
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+Berikut informasi Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=NXlxQUZUeHFQRXRtblBSWUdtalZFcUJVVkpINjVqWFpTL01WbGlMcE9yMzAxUnVaOXRnR0pNbFBvaG5TcVo5cU84V3RrTWhvNWMzQkpvWTgrOStQYjNNcGRlRXhURzhtdWxSNm9tN2taZk4zVnVHL212YzkrWGw1S3B2MnlRWW9KWGVFaWhwLzNWdVBQaXNhRUNOckU1ODJXRDU3eno2RkYwU2lEZy8xbjQvMkVWNmlWWDRWN1J4cTEveTkwQWlPVlZYNlU0L0VCWHF5WkkrYmNxNmpFTllYem41L3piQ1hFNW1POHFlWnhQOUVONVBMQWxTb0hWR0gvVks5ZkRlUTFOZmN4ZnVJTk9HM1pVdEpORWxHcTROL1RqdG1rUnNDWlV4aUMyMnVXVUU1K0NvUThkSSt6OUFVLzhtaHFMVFowNzhtaXRLYUlrdW9KUlJpb0o2ajdHUzB4M0sveXNqdlAxMGs5MDB4cjZNbVN1a1RMOWlQSHcyVnNPU1ZDZ0pmSE8rd2lUZDZJRlZXemQ1cmhnckJHQUludXZha3ZCZkwzU3BQTWZQRzFuU2dtaVdTMHp2VDM2VlNmaFk9)</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>IB6L42</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:17:30</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>200</v>
+      </c>
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30. Berikan 1 berita saja.
+###
+Answer:Salam Harmoni🙏
+Berita terbaru yang dapat saya sampaikan adalah sebagai berikut:
+**Judul:** FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak  
+**Tanggal Publikasi:** Rabu, 20 November 2024  
+**Deskripsi:** Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Universitas Pendidikan Ganesha (Undiksha) telah menyelenggarakan Focus Group Discussion (FGD) untuk mendukung peningkatan kesadaran gender dan perlindungan anak.  
+**Link:** [Baca Selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)
+Selain itu, kami mohon maaf bahwa pengajuan proses reset password untuk akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima menunjukkan bahwa email yang Anda gunakan tidak diizinkan untuk melakukan reset password. Silakan periksa kembali alamat email yang Anda masukkan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut. Terima kasih!
+Berikut informasi mengenai kelulusan peserta SMBJM di Undiksha (Universitas Pendidikan Ganesha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+Terakhir, berikut informasi Kartu Tanda Mahasiswa (KTM) Anda:
+- NIM: 2115101014
+- URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=Qk9iWUZIYkNyQXU2OXhLWEdsR2RBOVQ2MEpGdXloWFhYL1ZhcnNvN1dJK0VYQS8yUzRWOUc4eS9Eb2hsQWw3eTcwMXZQT1FmRW9yT0dQWWVXYWxqT0wyOERTMWtoaGlnWUVUbHVuS3I4U0ZWWG5FVHhFRVYzWTFiMElQVThId3FlY1NxbjNzNGttZkkwNmhhNEZCUDRrRVliSnVzUlNtc3Q4bGYrVWdKKzNXemNxTnFaQTh5MHRhS0xuWXhCR3Q3dzJTR2k2VUhzOS9pTXd4ZTh1MVhUaGtPYUlpUmxxTW4vMU9FNEN0bWZqbDYzMjZOc0w3YXVKYTFKRDllaWxQS3llUjBrWGpuM0xmN0YvbkVqVk1MNkVIVUhTVWFoKy9HaXhSWHJ3cDl4dlFxM2lBbnF6aStzYU5CNXlSM1NVdkRiUDFsMFBzbW44enJDNm5xMCtyQk1xV2xmS3JibW0yaGwrTGZNWi9OMVd4U1Y0TXRKQ0QwdkZzQWdxVkVGenl3Q3hqbGljZVdaZnZxVTk0OTBJQXpsWXRWMHFMbmkyZ2l0WUhhV1ZRclBtQUtweUhIQWRxQ1FQTGMxSzA9)
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>LKJ10B</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:18:38</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>200</v>
+      </c>
+      <c r="E143" t="b">
+        <v>1</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Berikan 1 berita saja. Saya lupa password sso email@undiksha.ac.id sudah ada akun google di hp. Cetak ktm 2115101014. Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi terbaru yang dapat saya sampaikan:
+1. **Berita Terbaru:**
+   - **Judul:** FGD dengan Pemkab Buleleng, Undiksha Dukung Peningkatan Kesadaran Gender dan Perlindungan Anak
+   - **Tanggal Publikasi:** Rabu, 20 November 2024
+   - **Deskripsi:** Pusat Kajian Gender dan Anak Lembaga Penelitian dan Pengabdian pada Masyarakat (LPPM) Universitas Pendidikan Ganesha (Undiksha) telah menyelenggarakan Focus Group.
+   - **Link:** [Baca Selengkapnya](https://undiksha.ac.id/fgd-dengan-pemkab-buleleng-undiksha-dukung-peningkatan-kesadaran-gender-dan-perlindungan-anak/)
+2. **Informasi Akun SSO E-Ganesha:**
+   - Pengajuan proses reset password akun SSO E-Ganesha Undiksha Anda tidak berhasil. Pesan kesalahan yang diterima adalah "Email ini tidak diizinkan." Silakan periksa kembali alamat email yang Anda gunakan atau hubungi pihak administrasi Undiksha untuk mendapatkan bantuan lebih lanjut.
+3. **Kelulusan Peserta SMBJM di Undiksha:**
+   - **Nomor Pendaftaran:** 3242000006
+   - **Nama Siswa:** KADEK YUNI SEDANI
+   - **Tanggal Lahir:** 30 November 2005
+   - **Tahun Daftar:** 2024
+   - **Pilihan Program Studi:** Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - **Status Kelulusan:** Lulus
+   - Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!
+4. **Informasi Kartu Tanda Mahasiswa (KTM):**
+   - **NIM:** 2115101014
+   - **URL KTM:** [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=VkRUU09GbHpLYlVodjd5WFB0c0RrMWdVRGxhNUNnRlU3Q21CR1FZVVR2VUFvcnJXMVg2R1h5OEQrMW9CS3NSWVpxZmI4azZGNkg5eHpyRklxQjdoOUtzUXdFNUpQYkg2QkNURjZ1R3FPNHRqS1MyK2F6N0RGNEZiUUFPQjlOZ0lPRGVsTjFhMkJyVTYrYjdmT2Mxb0ZsVzM0SmZEZE1NL1BNeko1VFMwZElQTnVRVTM0WkMzNWx1TVBFdVJoTHJuYjN1QXdBMXU5VGtGMFEwTVVuTFlENUlJT29KdU9RRjZLbGt6WTRnaXQ2bURRc2E5elpqL21tTkhQeDF6cWtLWlV2cGROK1FYTTdLaHlTREVEUUJKNkZKQ29hY1JqYkpmMWxiSkFLZGdabS8yOVNaY0phNE1QLzQxNzFPeDhPV3hRa2hUNS95TGVzNG96bnZ4a3hRc1BqM0RmUWczdFd2V3lwRWRFVW40OXpnS0wycnJLcE1EVjdlTW50bVJTTzFBTUVFYWVWODJuMlZSU1lRM0kvUzdKK2F5aGkyeGlwelpqYlVXSlB1RTQvdnhMa3FJVW5nQmg3RzE5STg9)
+5. **Rektor Universitas Pendidikan Ganesha:**
+   - Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>1CJ6TD</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:20:53</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>200</v>
+      </c>
+      <c r="E144" t="b">
+        <v>1</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:20:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>8IH50E</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:25:27</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>200</v>
+      </c>
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:25:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>KCRCHV</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:27:08</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>200</v>
+      </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:27:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>04V11R</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:27:08</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>200</v>
+      </c>
+      <c r="E147" t="b">
+        <v>1</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:27:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>NVP1UC</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:27:25</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>200</v>
+      </c>
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:27:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>HHQ30I</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:27:25</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>200</v>
+      </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:27:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>5URF7V</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:27:53</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>200</v>
+      </c>
+      <c r="E150" t="b">
+        <v>1</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Hai
+###
+Answer:Salam Harmoni🙏
+Halo! Saya Shavira, Ganesha Virtual Assistant dari Universitas Pendidikan Ganesha. Jika Anda memiliki pertanyaan terkait universitas atau informasi lainnya, silakan ajukan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>TZLA90</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:28:44</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>200</v>
+      </c>
+      <c r="E151" t="b">
+        <v>1</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:28:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>9P9K18</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:28:45</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>200</v>
+      </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:28:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>FJMJA2</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:29:10</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>200</v>
+      </c>
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:29:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>H5H3CA</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:29:10</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>200</v>
+      </c>
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:29:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>I8PBUL</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:29:35</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>200</v>
+      </c>
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:hai
+###
+Answer:Salam Harmoni🙏
+Halo! Saya Shavira, Ganesha Virtual Assistant dari Universitas Pendidikan Ganesha. Ada yang bisa saya bantu?</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>119ZDO</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:29:50</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>200</v>
+      </c>
+      <c r="E156" t="b">
+        <v>1</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:hai 2
+###
+Answer:Salam Harmoni🙏
+Halo! Ada yang bisa saya bantu terkait Universitas Pendidikan Ganesha?</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>0P27S2</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:29:56</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>200</v>
+      </c>
+      <c r="E157" t="b">
+        <v>1</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:29:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>WSN01S</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:29:56</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>200</v>
+      </c>
+      <c r="E158" t="b">
+        <v>1</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:29:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>IPCY1Y</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:17</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>200</v>
+      </c>
+      <c r="E159" t="b">
+        <v>1</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:30:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>1QB1AH</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:17</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>200</v>
+      </c>
+      <c r="E160" t="b">
+        <v>1</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:30:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>C74RAO</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:26</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>200</v>
+      </c>
+      <c r="E161" t="b">
+        <v>1</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Hai 1
+###
+Answer:Salam Harmoni🙏
+Halo! Saya Shavira, Ganesha Virtual Assistant dari Universitas Pendidikan Ganesha. Jika Anda memiliki pertanyaan terkait universitas atau informasi lainnya yang relevan, silakan ajukan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>3PYJBU</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:31</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>200</v>
+      </c>
+      <c r="E162" t="b">
+        <v>1</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:30:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>XKNQJA</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:31</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>200</v>
+      </c>
+      <c r="E163" t="b">
+        <v>1</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:30:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>GWKRFW</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:40</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>200</v>
+      </c>
+      <c r="E164" t="b">
+        <v>1</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Hai 2
+###
+Answer:Salam Harmoni🙏
+Halo! Saya Shavira, Ganesha Virtual Assistant dari Universitas Pendidikan Ganesha. Jika Anda memiliki pertanyaan terkait universitas atau informasi lainnya yang relevan, silakan ajukan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>KBYVWD</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:44</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>200</v>
+      </c>
+      <c r="E165" t="b">
+        <v>1</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:30:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>R72E00</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:30:44</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>200</v>
+      </c>
+      <c r="E166" t="b">
+        <v>1</v>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:30:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>DOGCQY</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:31:14</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>200</v>
+      </c>
+      <c r="E167" t="b">
+        <v>1</v>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-20 21:31:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>AL0TLK</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>2024-11-20 21:31:41</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>GET /datasets/list</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>200</v>
+      </c>
+      <c r="E168" t="b">
+        <v>1</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Datasets ditemukan.
+###
+Datasets:['Beasiswa.pdf', 'Daya Tampung Mahasiswa Baru.pdf', 'FAQ DOSEN.pdf', 'FAQ MAHASISWA.pdf', 'FAQ PENERIMAAN MAHASISWA SMBJM.pdf', 'FAQ REMUNERASI.pdf', 'FAQ UMUM.pdf', 'Fasilitas.pdf', 'FBS.pdf', 'FE.pdf', 'FHIS.pdf', 'FIP.pdf', 'FK.pdf', 'FMIPA.pdf', 'FOK.pdf', 'FTK.pdf', 'Jadwal PMB.pdf', 'Kurikulum.pdf', 'PANDUAN PENDAFTARAN KEMBALI SMBJM dengan skor UTBK-SNBT dan Prestasi-signed.pdf', 'Panduan-Pendaftaran-Kembali-SMBJM-CBT_2024rv1.pdf', 'Panduan-Pendaftaran-Kembali-SNBP-2024-v4-wa-signed.pdf', 'Panduan-Pendaftaran-Kembali-SNBT-2024_rev_signed.pdf', 'Pascasarjana.pdf', 'Pedoman-Studi-2017.pdf', 'Prosedur Pembayaran UKT.pdf', 'SMBJM.pdf', 'SNBP.pdf', 'SNBT.pdf', 'UKM.pdf', 'Umum.pdf', 'UPA TIK.pdf']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update: build new vector database
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F385"/>
+  <dimension ref="A1:F393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12670,6 +12670,246 @@
         </is>
       </c>
     </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>V4S75B</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:44:17</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D386" t="n">
+        <v>401</v>
+      </c>
+      <c r="E386" t="b">
+        <v>0</v>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>5IKUQO</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:44:17</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D387" t="n">
+        <v>404</v>
+      </c>
+      <c r="E387" t="b">
+        <v>0</v>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>HDEL6D</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:44:31</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D388" t="n">
+        <v>200</v>
+      </c>
+      <c r="E388" t="b">
+        <v>1</v>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:44:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>SWSD4G</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:45:16</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>GET /checkmodel</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>200</v>
+      </c>
+      <c r="E389" t="b">
+        <v>1</v>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>OK
+###
+Log Config LLM:{'last_update': '2024-11-17 20:22:21', 'llm': 'openai', 'model_llm': 'gpt-4o', 'embbeder': 'openai', 'model_embedder': 'text-embedding-3-large', 'chunk_size': 1000, 'chunk_overlap': 200, 'total_chunks': 1023}</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>PN9IYD</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:45:34</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>400</v>
+      </c>
+      <c r="E390" t="b">
+        <v>0</v>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>Embedder harus 'openai' atau 'ollama'.</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>GP1KBH</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:48:45</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D391" t="n">
+        <v>400</v>
+      </c>
+      <c r="E391" t="b">
+        <v>0</v>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>Embedder harus 'openai' atau 'ollama'.</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>EG78BY</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:48:52</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D392" t="n">
+        <v>400</v>
+      </c>
+      <c r="E392" t="b">
+        <v>0</v>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>Model Embedder untuk 'openai' harus salah satu dari ['text-embedding-3-large', 'text-embedding-3-small'].</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>QKF843</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:49:52</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>200</v>
+      </c>
+      <c r="E393" t="b">
+        <v>1</v>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embbeder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:1000</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update: try to fix date or timezone api
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F393"/>
+  <dimension ref="A1:F434"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12910,6 +12910,1156 @@
         </is>
       </c>
     </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>I3KNC0</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:06:24</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D394" t="n">
+        <v>401</v>
+      </c>
+      <c r="E394" t="b">
+        <v>0</v>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>MLUJ5S</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:06:24</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D395" t="n">
+        <v>404</v>
+      </c>
+      <c r="E395" t="b">
+        <v>0</v>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>BBIG20</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:06:37</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D396" t="n">
+        <v>200</v>
+      </c>
+      <c r="E396" t="b">
+        <v>1</v>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:06:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>B4IT6K</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:06:53</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D397" t="n">
+        <v>200</v>
+      </c>
+      <c r="E397" t="b">
+        <v>1</v>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:06:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>PD78F5</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:06:56</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D398" t="n">
+        <v>200</v>
+      </c>
+      <c r="E398" t="b">
+        <v>1</v>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:06:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>LBG84X</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:18</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D399" t="n">
+        <v>200</v>
+      </c>
+      <c r="E399" t="b">
+        <v>1</v>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>HV2TCV</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:19</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>200</v>
+      </c>
+      <c r="E400" t="b">
+        <v>1</v>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>NLFWZ4</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:19</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D401" t="n">
+        <v>200</v>
+      </c>
+      <c r="E401" t="b">
+        <v>1</v>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>YBRISH</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:20</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D402" t="n">
+        <v>200</v>
+      </c>
+      <c r="E402" t="b">
+        <v>1</v>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>OY0BNU</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:20</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
+        <v>200</v>
+      </c>
+      <c r="E403" t="b">
+        <v>1</v>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>6M3GHU</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:21</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D404" t="n">
+        <v>200</v>
+      </c>
+      <c r="E404" t="b">
+        <v>1</v>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>8ZEA8Z</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:21</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D405" t="n">
+        <v>200</v>
+      </c>
+      <c r="E405" t="b">
+        <v>1</v>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>19YEPX</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:21</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D406" t="n">
+        <v>200</v>
+      </c>
+      <c r="E406" t="b">
+        <v>1</v>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>3X854H</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:29</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D407" t="n">
+        <v>200</v>
+      </c>
+      <c r="E407" t="b">
+        <v>1</v>
+      </c>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>9CGKO1</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:10:30</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D408" t="n">
+        <v>200</v>
+      </c>
+      <c r="E408" t="b">
+        <v>1</v>
+      </c>
+      <c r="F408" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>RJ4P7W</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:20:10</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D409" t="n">
+        <v>200</v>
+      </c>
+      <c r="E409" t="b">
+        <v>1</v>
+      </c>
+      <c r="F409" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:20:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>KVITQC</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:24:32</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D410" t="n">
+        <v>200</v>
+      </c>
+      <c r="E410" t="b">
+        <v>1</v>
+      </c>
+      <c r="F410" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:24:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>CX6JB8</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:25:25</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>200</v>
+      </c>
+      <c r="E411" t="b">
+        <v>1</v>
+      </c>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:25:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>C85Y1Q</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:25:33</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D412" t="n">
+        <v>200</v>
+      </c>
+      <c r="E412" t="b">
+        <v>1</v>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:25:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>0OIR6R</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:25:34</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D413" t="n">
+        <v>200</v>
+      </c>
+      <c r="E413" t="b">
+        <v>1</v>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:25:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>UECCLM</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:26:43</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D414" t="n">
+        <v>200</v>
+      </c>
+      <c r="E414" t="b">
+        <v>1</v>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:26:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>R9YFUY</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:26:51</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D415" t="n">
+        <v>200</v>
+      </c>
+      <c r="E415" t="b">
+        <v>1</v>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 19:26:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>4P1D98</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>2024-11-22 19:27:21</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>GET /datasets/list</t>
+        </is>
+      </c>
+      <c r="D416" t="n">
+        <v>200</v>
+      </c>
+      <c r="E416" t="b">
+        <v>1</v>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>Datasets ditemukan.
+###
+Datasets:['Beasiswa.pdf', 'Daya Tampung Mahasiswa Baru.pdf', 'FAQ DOSEN.pdf', 'FAQ MAHASISWA.pdf', 'FAQ PENERIMAAN MAHASISWA SMBJM.pdf', 'FAQ REMUNERASI.pdf', 'FAQ UMUM.pdf', 'Fasilitas.pdf', 'FBS.pdf', 'FE.pdf', 'FHIS.pdf', 'FIP.pdf', 'FK.pdf', 'FMIPA.pdf', 'FOK.pdf', 'FTK.pdf', 'Jadwal PMB.pdf', 'Kurikulum.pdf', 'PANDUAN PENDAFTARAN KEMBALI SMBJM dengan skor UTBK-SNBT dan Prestasi-signed.pdf', 'Panduan-Pendaftaran-Kembali-SMBJM-CBT_2024rv1.pdf', 'Panduan-Pendaftaran-Kembali-SNBP-2024-v4-wa-signed.pdf', 'Panduan-Pendaftaran-Kembali-SNBT-2024_rev_signed.pdf', 'Pascasarjana.pdf', 'Pedoman-Studi-2017.pdf', 'Prosedur Pembayaran UKT.pdf', 'SMBJM.pdf', 'SNBP.pdf', 'SNBT.pdf', 'UKM.pdf', 'Umum.pdf', 'UPA TIK.pdf']</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>0ZBJ7W</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:27:54</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D417" t="n">
+        <v>200</v>
+      </c>
+      <c r="E417" t="b">
+        <v>1</v>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:27:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>T7R75F</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:29:11</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D418" t="n">
+        <v>200</v>
+      </c>
+      <c r="E418" t="b">
+        <v>1</v>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:29:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>8WRJI1</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:29:14</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D419" t="n">
+        <v>200</v>
+      </c>
+      <c r="E419" t="b">
+        <v>1</v>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:29:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>QFG9KH</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:10</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D420" t="n">
+        <v>200</v>
+      </c>
+      <c r="E420" t="b">
+        <v>1</v>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>ABY6TG</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:12</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D421" t="n">
+        <v>200</v>
+      </c>
+      <c r="E421" t="b">
+        <v>1</v>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>4UEU7C</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:12</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D422" t="n">
+        <v>200</v>
+      </c>
+      <c r="E422" t="b">
+        <v>1</v>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>O92CB0</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:13</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D423" t="n">
+        <v>200</v>
+      </c>
+      <c r="E423" t="b">
+        <v>1</v>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>F5PRKE</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:13</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D424" t="n">
+        <v>200</v>
+      </c>
+      <c r="E424" t="b">
+        <v>1</v>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>ZA20DR</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:14</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D425" t="n">
+        <v>200</v>
+      </c>
+      <c r="E425" t="b">
+        <v>1</v>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>RB2EC4</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:49</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D426" t="n">
+        <v>200</v>
+      </c>
+      <c r="E426" t="b">
+        <v>1</v>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>SXPMBM</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:30:50</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D427" t="n">
+        <v>200</v>
+      </c>
+      <c r="E427" t="b">
+        <v>1</v>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:30:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>UMF3VX</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:32:47</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D428" t="n">
+        <v>401</v>
+      </c>
+      <c r="E428" t="b">
+        <v>0</v>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>MZYR0S</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:32:47</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D429" t="n">
+        <v>404</v>
+      </c>
+      <c r="E429" t="b">
+        <v>0</v>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>D6GIIX</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:32:48</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D430" t="n">
+        <v>401</v>
+      </c>
+      <c r="E430" t="b">
+        <v>0</v>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>KE2DNM</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:33:00</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D431" t="n">
+        <v>200</v>
+      </c>
+      <c r="E431" t="b">
+        <v>1</v>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:33:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>Q5CLLD</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:36:33</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D432" t="n">
+        <v>401</v>
+      </c>
+      <c r="E432" t="b">
+        <v>0</v>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>K3UBQV</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:36:51</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D433" t="n">
+        <v>200</v>
+      </c>
+      <c r="E433" t="b">
+        <v>1</v>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:36:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>C3LMV9</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>2024-11-22 21:37:35</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D434" t="n">
+        <v>200</v>
+      </c>
+      <c r="E434" t="b">
+        <v>1</v>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-22 21:37:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update: fix clean code
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F434"/>
+  <dimension ref="A1:F465"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14060,6 +14060,1147 @@
         </is>
       </c>
     </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>E1DLN0</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:06:47</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D435" t="n">
+        <v>401</v>
+      </c>
+      <c r="E435" t="b">
+        <v>0</v>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>61YFI0</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:06:47</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D436" t="n">
+        <v>404</v>
+      </c>
+      <c r="E436" t="b">
+        <v>0</v>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>D5DIIV</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:07:05</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D437" t="n">
+        <v>200</v>
+      </c>
+      <c r="E437" t="b">
+        <v>1</v>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-23 21:07:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>FM86LE</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:07:05</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D438" t="n">
+        <v>200</v>
+      </c>
+      <c r="E438" t="b">
+        <v>1</v>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-23 21:07:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>4SBL6J</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:07:15</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D439" t="n">
+        <v>200</v>
+      </c>
+      <c r="E439" t="b">
+        <v>1</v>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Berikut adalah informasi yang Anda berikan:
+- Email Account User: Tidak disebutkan
+- Login Account Status: Belum login
+Petunjuk untuk Pengguna:
+- Pastikan Anda menggunakan email valid dari Undiksha, yaitu yang berakhiran "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google Anda sudah login di email/gmail/google/hp/laptop/komputer.
+Silakan periksa kembali informasi yang Anda berikan dan coba lagi. Terima kasih!</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>GUQAZL</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:09:43</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D440" t="n">
+        <v>200</v>
+      </c>
+      <c r="E440" t="b">
+        <v>1</v>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:saya lupa akun
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses mengenai akun SSO E-Ganesha atau Google Undiksha Anda terdapat anomali. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk memproses akun Anda. 
+Atau Anda dapat mengecek pada kontak berikut untuk informasi lebih lanjut: [https://upttik.undiksha.ac.id/kontak-kami](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>432MEQ</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:11:17</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D441" t="n">
+        <v>200</v>
+      </c>
+      <c r="E441" t="b">
+        <v>1</v>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:saya lupa akun
+###
+Answer:Salam Harmoni🙏
+Jika Anda lupa akun, Anda dapat mencoba langkah-langkah berikut:
+1. **Cek Email**: Periksa email yang mungkin Anda gunakan untuk mendaftar. Cari email konfirmasi atau informasi akun dari Universitas Pendidikan Ganesha.
+2. **Reset Password**: Jika Anda ingat username tetapi lupa password, coba gunakan opsi "Lupa Password" pada halaman login.
+3. **Hubungi UPT TIK**: Jika Anda tidak dapat menemukan informasi akun Anda, silakan hubungi UPT TIK untuk mendapatkan bantuan lebih lanjut. Mereka dapat membantu Anda memeriksa status akun dan memberikan solusi.
+Pastikan untuk memberikan informasi yang diperlukan saat menghubungi mereka agar prosesnya lebih cepat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>O0KAK6</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:12:09</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D442" t="n">
+        <v>200</v>
+      </c>
+      <c r="E442" t="b">
+        <v>1</v>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:saya lupa akun
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO E-Ganesha atau Google Undiksha Anda. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk mengurus akun Anda. Atau Anda dapat mengecek informasi lebih lanjut pada kontak yang tersedia di [sini](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>SJ4Y7M</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:12:35</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D443" t="n">
+        <v>200</v>
+      </c>
+      <c r="E443" t="b">
+        <v>1</v>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO E-Ganesha atau Google Undiksha Anda. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk mengurus akun Anda. Atau Anda dapat mengecek informasi lebih lanjut pada kontak yang tersedia di [sini](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>GO23O3</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:13:23</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D444" t="n">
+        <v>200</v>
+      </c>
+      <c r="E444" t="b">
+        <v>1</v>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO E-Ganesha atau Google Undiksha Anda. Silahkan datang langsung ke Kantor UPA TIK Undiksha untuk mengurus akun Anda. Atau Anda dapat mengecek informasi lebih lanjut pada kontak kami di [https://upttik.undiksha.ac.id/kontak-kami](https://upttik.undiksha.ac.id/kontak-kami).</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>YLBZKZ</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:13:46</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D445" t="n">
+        <v>200</v>
+      </c>
+      <c r="E445" t="b">
+        <v>1</v>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Berikut adalah informasi yang diberikan:
+- **Email Account User**: Tidak disebutkan
+- **Login Account Status**: Belum login
+Petunjuk untuk Pengguna:
+- Pastikan Anda menggunakan email valid dari Undiksha, yaitu "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google Anda sudah login di email/gmail/google/hp/laptop/komputer.
+Kesalahan pengguna: Anda belum menyebutkan email dan status login Anda.
+Silakan mengisi format pengajuan berikut:
+- **Email**: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- **Login Status**: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>X58WV6</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:14:30</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D446" t="n">
+        <v>200</v>
+      </c>
+      <c r="E446" t="b">
+        <v>1</v>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Berikut adalah informasi yang diberikan:
+- Email Account User: Tidak disebutkan
+- Login Account Status: Belum login
+Petunjuk untuk Anda:
+- Pastikan menggunakan email valid dari Undiksha, yaitu yang berakhiran "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google Anda sudah login di email/gmail/google/hp/laptop/komputer.
+Silakan mengisi format pengajuan berikut:
+- Email: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- Login Status: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>FARSGM</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:15:13</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D447" t="n">
+        <v>200</v>
+      </c>
+      <c r="E447" t="b">
+        <v>1</v>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, pengajuan proses reset password akun SSO E-Ganesha Undiksha tidak berhasil. Berikut adalah informasi yang diberikan:
+- **Email Account User**: Tidak disebutkan
+- **Login Account Status**: Belum login
+Petunjuk untuk Pengguna:
+- Pastikan Anda menggunakan email valid dari Undiksha, yaitu yang berakhiran "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google Anda sudah login di email/gmail/google/hp/laptop/komputer.
+Silakan mengisi format pengajuan berikut:
+- **Email**: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- **Login Status**: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>NLLC14</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:16:44</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D448" t="n">
+        <v>200</v>
+      </c>
+      <c r="E448" t="b">
+        <v>1</v>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO E-Ganesha atau Google Undiksha Anda. Berikut adalah informasi yang diberikan:
+- **Email Account User**: Tidak disebutkan
+- **Login Account Status**: Belum login
+Petunjuk untuk Pengguna:
+- Pastikan Anda menggunakan email valid dari Undiksha, yaitu "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google sudah login di email/gmail/google/hp/laptop/komputer.
+Silakan periksa kembali informasi Anda dan beritahu jika ada kesalahan.
+Minta Pengguna untuk Mengisi Format Pengajuan:
+- **Email**: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- **Login Status**: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>7DJI56</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:17:34</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D449" t="n">
+        <v>200</v>
+      </c>
+      <c r="E449" t="b">
+        <v>1</v>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO E-Ganesha atau Google Undiksha Anda. Berikut adalah informasi yang diberikan:
+- Email Account User: Tidak disebutkan
+- Login Account Status: Belum login
+Petunjuk untuk Anda:
+- Pastikan email yang Anda gunakan valid dari Undiksha, yaitu "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google sudah login di email/gmail/google/hp/laptop/komputer.
+Jika Anda ingin melakukan reset password, silakan isi format pengajuan berikut:
+- Email: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- Login Status: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>77PTPK</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:18:19</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D450" t="n">
+        <v>200</v>
+      </c>
+      <c r="E450" t="b">
+        <v>1</v>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO E-Ganesha atau Google Undiksha Anda. Berikut adalah informasi yang diberikan:
+- Email Account User: Tidak disebutkan
+- Login Account Status: Belum login
+Petunjuk untuk Anda:
+- Pastikan Anda menggunakan email valid dari Undiksha, yaitu "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google Anda sudah login di email/gmail/google/hp/laptop/komputer.
+Jika Anda ingin melakukan reset password, silakan isi format pengajuan berikut dan kirim di sini:
+- Email: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- Login Status: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>5USTDT</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:21:30</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D451" t="n">
+        <v>200</v>
+      </c>
+      <c r="E451" t="b">
+        <v>1</v>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO atau Google Undiksha Anda. Berikut informasi yang diberikan:
+- Email Account User: Tidak disebutkan
+- Login Account Status: Belum login
+Petunjuk untuk Anda:
+- Pastikan Anda menggunakan email valid dari Undiksha, yaitu "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google Anda sudah login di email/gmail/google/hp/laptop/komputer.
+Jika Anda ingin melakukan reset password, silakan isi format pengajuan berikut dan kirim di sini:
+- Email: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- Login Status: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>JENR5V</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:22:17</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D452" t="n">
+        <v>200</v>
+      </c>
+      <c r="E452" t="b">
+        <v>1</v>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya lupa password SSO Undiksha.
+###
+Answer:Salam Harmoni🙏
+Mohon maaf, saya tidak dapat membantu menangani akun SSO atau Google Undiksha Anda. Berikut informasi yang Anda berikan:
+- Email Account User: Tidak disebutkan
+- Login Account Status: Belum login
+Petunjuk untuk Anda:
+- Pastikan Anda menggunakan email valid dari Undiksha, yaitu "@undiksha.ac.id" atau "@student.undiksha.ac.id".
+- Pastikan akun Google Anda sudah login di email/gmail/google/hp/laptop/komputer.
+Jika Anda ingin mereset password, silakan isi format pengajuan berikut dan kirim di sini:
+- Email: Masukkan Email (contoh: shavira@undiksha.ac.id atau shavira@student.undiksha.ac.id)
+- Login Status: Masukkan Status Login (Contoh: Sudah Login / Belum Login di Perangkat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>BD3VXH</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:22:40</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D453" t="n">
+        <v>200</v>
+      </c>
+      <c r="E453" t="b">
+        <v>1</v>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya ingin cek kelulusan pendaftaran.
+###
+Answer:Salam Harmoni🙏
+Dari informasi yang ada, saat ini belum terdapat Nomor Pendaftaran dan Tanggal Lahir Pendaftar SMBJM yang diberikan. Untuk melakukan pengecekan kelulusan, Anda perlu mengikuti format penulisan pesan yang telah ditentukan. 
+Format penulisan pesan adalah sebagai berikut:
+Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
+Sebagai contoh, penulisan pesan yang benar adalah:
+Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
+Pastikan untuk mengirimkan pesan sesuai dengan format dan contoh yang telah diberikan agar dapat mengecek kelulusan SMBJM Undiksha dengan benar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>ODOGME</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:23:09</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D454" t="n">
+        <v>200</v>
+      </c>
+      <c r="E454" t="b">
+        <v>1</v>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cara akses melihat KTM.
+###
+Answer:Salam Harmoni🙏
+Dari informasi yang ada, saat ini belum terdapat nomor NIM (Nomor Induk Mahasiswa) yang diberikan. NIM yang valid dari Undiksha terdiri dari 10 digit angka. Untuk penulisan pesan, format yang harus digunakan adalah sebagai berikut:
+KTM [NIM]
+Sebagai contoh, penulisan pesan yang benar adalah:
+KTM 1234567890
+Silakan kirimkan NIM yang benar pada pesan ini sesuai dengan format dan contoh yang telah diberikan, agar proses pencetakan Kartu Tanda Mahasiswa (KTM) dapat dilakukan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>N9G198</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:26:10</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D455" t="n">
+        <v>200</v>
+      </c>
+      <c r="E455" t="b">
+        <v>1</v>
+      </c>
+      <c r="F455" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cara akses melihat KTM.
+###
+Answer:Salam Harmoni🙏
+Untuk melihat Kartu Tanda Mahasiswa (KTM), Anda perlu mengirimkan NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Berikut adalah format penulisan pesan yang harus diikuti:
+- Format penulisan pesan: KTM [NIM]
+- Contoh penulisan pesan: KTM 1234567890
+Pastikan Anda mengirimkan NIM yang benar sesuai dengan format dan contoh di atas agar dapat melihat KTM Anda.</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>AU6KI4</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:26:50</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D456" t="n">
+        <v>200</v>
+      </c>
+      <c r="E456" t="b">
+        <v>1</v>
+      </c>
+      <c r="F456" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cara akses melihat KTM.
+###
+Answer:Salam Harmoni🙏
+Untuk melihat Kartu Tanda Mahasiswa (KTM), Anda dapat melakukannya melalui SSO Undiksha atau dengan mengirimkan pesan. Namun, Anda perlu mengirimkan NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Berikut adalah format penulisan pesan yang harus diikuti:
+- Format penulisan pesan: KTM [NIM]
+- Contoh penulisan pesan: KTM 1234567890
+Pastikan untuk mengirimkan NIM yang benar sesuai dengan format dan contoh di atas agar Anda dapat melihat KTM Anda.</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>L7ZZCH</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:27:05</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D457" t="n">
+        <v>200</v>
+      </c>
+      <c r="E457" t="b">
+        <v>1</v>
+      </c>
+      <c r="F457" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cara akses melihat KTM.
+###
+Answer:Salam Harmoni🙏
+Untuk melihat Kartu Tanda Mahasiswa (KTM), Anda dapat melakukannya melalui SSO Undiksha atau dengan mengirimkan pesan. Namun, Anda perlu mengirimkan NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Berikut adalah format penulisan pesan yang harus diikuti:
+- Format penulisan pesan: KTM [NIM]
+- Contoh penulisan pesan: KTM 1234567890
+Pastikan untuk mengirimkan NIM yang benar sesuai dengan format dan contoh di atas agar Anda dapat melihat KTM Anda.</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>OZPDL9</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:27:23</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D458" t="n">
+        <v>200</v>
+      </c>
+      <c r="E458" t="b">
+        <v>1</v>
+      </c>
+      <c r="F458" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cara akses melihat KTM.
+###
+Answer:Salam Harmoni🙏
+Untuk melihat Kartu Tanda Mahasiswa (KTM), Anda dapat melakukannya melalui SSO Undiksha atau melalui pesan. Namun, Anda perlu mengirimkan NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Berikut adalah format penulisan pesan yang harus diikuti:
+- Format penulisan pesan: KTM [NIM]
+- Contoh penulisan pesan: KTM 1234567890
+Pastikan NIM yang Anda kirimkan adalah benar agar dapat mengakses KTM dengan tepat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>MABB4H</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:28:00</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D459" t="n">
+        <v>200</v>
+      </c>
+      <c r="E459" t="b">
+        <v>1</v>
+      </c>
+      <c r="F459" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cara akses melihat KTM.
+###
+Answer:Salam Harmoni🙏
+Untuk melihat Kartu Tanda Mahasiswa (KTM), Anda dapat mengaksesnya melalui SSO Undiksha atau melalui tautan yang disediakan. Namun, Anda perlu mengirimkan NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Berikut adalah format penulisan pesan yang harus Anda ikuti:
+- Format penulisan pesan: KTM [NIM]
+- Contoh penulisan pesan: KTM 1234567890
+Pastikan NIM yang Anda kirimkan adalah benar agar dapat mengakses KTM dengan lancar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>6LZBBC</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:28:44</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D460" t="n">
+        <v>200</v>
+      </c>
+      <c r="E460" t="b">
+        <v>1</v>
+      </c>
+      <c r="F460" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cara akses melihat KTM.
+###
+Answer:Salam Harmoni🙏
+Untuk melihat Kartu Tanda Mahasiswa (KTM), Anda dapat melakukannya melalui SSO Undiksha atau dengan mengirimkan pesan. Jika Anda memilih untuk mengirimkan pesan, Anda perlu menyertakan NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Berikut adalah format penulisan pesan yang harus Anda ikuti:
+- KTM [NIM]
+Contoh penulisan pesan yang benar:
+- KTM 1234567890
+Silakan kirimkan NIM Anda untuk mendapatkan informasi lebih lanjut mengenai KTM.</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>TF3MSD</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:29:08</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D461" t="n">
+        <v>200</v>
+      </c>
+      <c r="E461" t="b">
+        <v>1</v>
+      </c>
+      <c r="F461" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:2115101014
+###
+Answer:Salam Harmoni🙏
+Untuk melihat Kartu Tanda Mahasiswa (KTM), Anda dapat melakukannya melalui SSO Undiksha atau dengan mengirimkan pesan kepada saya. Namun, untuk itu diperlukan NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Berikut adalah format penulisan pesan yang harus Anda ikuti:
+- KTM [NIM]
+Contoh penulisan pesan yang benar:
+- KTM 1234567890
+Silakan kirimkan NIM Anda untuk mendapatkan informasi lebih lanjut mengenai KTM.</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>O3E6UC</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:29:47</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D462" t="n">
+        <v>200</v>
+      </c>
+      <c r="E462" t="b">
+        <v>1</v>
+      </c>
+      <c r="F462" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya ingin cek kelulusan pendaftaran.
+###
+Answer:Salam Harmoni🙏
+Dari informasi yang ada, belum terdapat Nomor Pendaftaran dan Tanggal Lahir Pendaftar SMBJM yang diberikan. Untuk melakukan pengecekan kelulusan, Anda perlu mengikuti format penulisan pesan yang telah ditentukan. 
+Format penulisan pesan adalah sebagai berikut:
+Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
+Sebagai contoh, penulisan pesan yang benar adalah:
+Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
+Pastikan untuk mengirimkan pesan sesuai dengan format dan contoh yang telah diberikan, agar Anda dapat mengecek kelulusan SMBJM Undiksha dengan benar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>6DWBE5</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:31:54</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D463" t="n">
+        <v>200</v>
+      </c>
+      <c r="E463" t="b">
+        <v>1</v>
+      </c>
+      <c r="F463" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya ingin cek kelulusan pendaftaran.
+###
+Answer:Salam Harmoni🙏
+Untuk mengecek kelulusan, Anda dapat mengunjungi link berikut: [https://penerimaan.undiksha.ac.id/smbjm/login](https://penerimaan.undiksha.ac.id/smbjm/login). Jika Anda ingin saya membantu, silakan kirimkan Nomor Pendaftaran dan Tanggal Lahir Anda untuk Pendaftar SMBJM.
+Berikut adalah format penulisan pesan yang perlu Anda ikuti:
+- Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
+Contoh penulisan pesan yang benar:
+- Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
+Silakan kirimkan informasi tersebut jika Anda memerlukan bantuan lebih lanjut.</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>72OCM8</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:33:15</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D464" t="n">
+        <v>200</v>
+      </c>
+      <c r="E464" t="b">
+        <v>1</v>
+      </c>
+      <c r="F464" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Saya ingin cek kelulusan pendaftaran.
+###
+Answer:Salam Harmoni🙏
+Untuk mengecek kelulusan, Anda dapat mengunjungi link berikut: [https://penerimaan.undiksha.ac.id/smbjm/login](https://penerimaan.undiksha.ac.id/smbjm/login). Jika Anda ingin, saya juga dapat membantu Anda melalui pesan ini. Namun, Anda perlu mengirimkan informasi berikut: Nomor Pendaftaran dan Tanggal Lahir Pendaftar SMBJM.
+Berikut adalah format penulisan pesan yang harus Anda ikuti:
+- Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
+Contoh penulisan pesan yang benar:
+- Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
+Silakan kirimkan informasi tersebut untuk mendapatkan bantuan lebih lanjut.</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>BR2CP7</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>2024-11-23 21:33:44</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D465" t="n">
+        <v>200</v>
+      </c>
+      <c r="E465" t="b">
+        <v>1</v>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30.
+###
+Answer:Salam Harmoni🙏
+Berikut informasi Kelulusan Peserta SMBJM di Undiksha (Universitas Pendidikan Ganesha):
+- Nomor Pendaftaran: 3242000006
+- Nama Siswa: KADEK YUNI SEDANI
+- Tanggal Lahir: 30 November 2005
+- Tahun Daftar: 2024
+- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+- Status Kelulusan: Lulus
+Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI! Semoga sukses dalam perjalanan akademik yang akan datang.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update: adding endpoint logs activity
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F500"/>
+  <dimension ref="A1:F507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17307,6 +17307,204 @@
         </is>
       </c>
     </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>PDEG0E</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>2024-12-02 09:23:30</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D501" t="n">
+        <v>401</v>
+      </c>
+      <c r="E501" t="b">
+        <v>0</v>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>2LBC23</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>2024-12-02 09:23:31</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D502" t="n">
+        <v>404</v>
+      </c>
+      <c r="E502" t="b">
+        <v>0</v>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>MZZ1AK</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>2024-12-02 09:28:16</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D503" t="n">
+        <v>200</v>
+      </c>
+      <c r="E503" t="b">
+        <v>1</v>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-12-02 09:28:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>BLAUVW</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>2024-12-02 09:28:30</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>GET /logs</t>
+        </is>
+      </c>
+      <c r="D504" t="n">
+        <v>200</v>
+      </c>
+      <c r="E504" t="b">
+        <v>1</v>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>application/vnd.openxmlformats-officedocument.spreadsheetml.sheet
+###
+filename=api/logs/log_activity.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>WXSUJ3</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>2024-12-02 09:37:39</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>GET /logs</t>
+        </is>
+      </c>
+      <c r="D505" t="n">
+        <v>200</v>
+      </c>
+      <c r="E505" t="b">
+        <v>1</v>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>Mengambil data log sebagai JSON</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>7TD7QV</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>2024-12-02 09:40:23</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>GET /logs</t>
+        </is>
+      </c>
+      <c r="D506" t="n">
+        <v>200</v>
+      </c>
+      <c r="E506" t="b">
+        <v>1</v>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>Mengambil data log sebagai JSON</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>JBAQ9Q</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>2024-12-02 09:42:04</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>GET /logs</t>
+        </is>
+      </c>
+      <c r="D507" t="n">
+        <v>200</v>
+      </c>
+      <c r="E507" t="b">
+        <v>1</v>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>Mengambil data log sebagai JSON</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: change the datasets 2024 to 2025 for SNBT and SNBP informations
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F524"/>
+  <dimension ref="A1:F528"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18053,6 +18053,132 @@
         </is>
       </c>
     </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>OEHAX3</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>2024-12-23 10:46:41</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D525" t="n">
+        <v>401</v>
+      </c>
+      <c r="E525" t="b">
+        <v>0</v>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1DSX09</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>2024-12-23 10:46:42</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D526" t="n">
+        <v>404</v>
+      </c>
+      <c r="E526" t="b">
+        <v>0</v>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>XGCJLB</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>2024-12-23 10:47:31</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D527" t="n">
+        <v>400</v>
+      </c>
+      <c r="E527" t="b">
+        <v>0</v>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>Model Embedder untuk 'openai' harus salah satu dari ['text-embedding-3-large', 'text-embedding-3-small'].</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>7OT3IV</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>2024-12-23 10:47:40</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D528" t="n">
+        <v>200</v>
+      </c>
+      <c r="E528" t="b">
+        <v>1</v>
+      </c>
+      <c r="F528" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embedder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:1129</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: remove dataset SMBJM 2024 and pendaftaran kembali SNBT. SNBP, SMBJM 2024, and change the faiss vectordb
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F528"/>
+  <dimension ref="A1:F529"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18179,6 +18179,48 @@
         </is>
       </c>
     </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>JFVZIE</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>2024-12-23 11:01:19</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D529" t="n">
+        <v>200</v>
+      </c>
+      <c r="E529" t="b">
+        <v>1</v>
+      </c>
+      <c r="F529" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embedder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:1061</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: change datasets umum
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F529"/>
+  <dimension ref="A1:F530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18221,6 +18221,48 @@
         </is>
       </c>
     </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>0GL5NJ</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>2024-12-23 11:18:12</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D530" t="n">
+        <v>200</v>
+      </c>
+      <c r="E530" t="b">
+        <v>1</v>
+      </c>
+      <c r="F530" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embedder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:1060</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: remove information pmb in kalender akademik 2024-2025 beacuse not used
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F530"/>
+  <dimension ref="A1:F531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18263,6 +18263,48 @@
         </is>
       </c>
     </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>CLS7KG</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>2024-12-23 11:33:08</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D531" t="n">
+        <v>200</v>
+      </c>
+      <c r="E531" t="b">
+        <v>1</v>
+      </c>
+      <c r="F531" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embedder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:1057</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: change the information in dataset umum
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F531"/>
+  <dimension ref="A1:F535"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18305,6 +18305,155 @@
         </is>
       </c>
     </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>FLJOE5</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>2024-12-23 11:35:38</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D532" t="n">
+        <v>200</v>
+      </c>
+      <c r="E532" t="b">
+        <v>1</v>
+      </c>
+      <c r="F532" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal penerimaan mahasiswa undiksha 2025?
+###
+Answer:Salam Harmoni🙏
+Jadwal penerimaan mahasiswa Universitas Pendidikan Ganesha (Undiksha) untuk tahun akademik 2024/2025 belum diumumkan secara resmi. Namun, biasanya informasi mengenai jadwal penerimaan mahasiswa akan diumumkan melalui situs resmi Undiksha atau media sosial resmi mereka. Disarankan untuk selalu memantau informasi terbaru dari sumber resmi untuk mendapatkan jadwal yang akurat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>WXCZAG</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>2024-12-23 11:36:12</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D533" t="n">
+        <v>200</v>
+      </c>
+      <c r="E533" t="b">
+        <v>1</v>
+      </c>
+      <c r="F533" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal penerimaan mahasiswa undiksha 2025?
+###
+Answer:Salam Harmoni🙏
+Jadwal penerimaan mahasiswa Universitas Pendidikan Ganesha (Undiksha) untuk tahun akademik 2024/2025 belum diumumkan secara resmi. Namun, biasanya informasi mengenai jadwal penerimaan mahasiswa akan diumumkan melalui situs resmi Undiksha atau media sosial resmi mereka. Disarankan untuk selalu memantau informasi terbaru dari sumber resmi tersebut. Jika ada pertanyaan lebih lanjut, silakan tanyakan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>KSEMJV</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>2024-12-23 11:36:50</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D534" t="n">
+        <v>200</v>
+      </c>
+      <c r="E534" t="b">
+        <v>1</v>
+      </c>
+      <c r="F534" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal snbp?
+###
+Answer:Salam Harmoni🙏
+Jadwal pelaksanaan Seleksi Nasional Berbasis Prestasi (SNBP) adalah sebagai berikut:
+1. Pengumuman Kuota Sekolah: 28 Desember 2024
+2. Masa Sanggah: 28 Desember 2024 – 17 Januari 2025
+3. Registrasi Akun SNPMB Sekolah: 6 – 31 Januari 2025
+4. Registrasi Akun SNPMB Siswa: 13 Januari – 18 Februari 2025
+5. Pendaftaran SNBP oleh Siswa: 4 – 18 Februari 2025
+6. Pengumuman Hasil SNBP: 18 Maret 2025
+7. Masa Unduh Kartu Peserta SNBP: 4 Februari – 30 April 2025
+Jika ada pertanyaan lebih lanjut, silakan tanyakan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>EPMVED</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>2024-12-23 11:40:04</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D535" t="n">
+        <v>200</v>
+      </c>
+      <c r="E535" t="b">
+        <v>1</v>
+      </c>
+      <c r="F535" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embedder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:1057</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: update datasets and rebuild vectordb
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F535"/>
+  <dimension ref="A1:F549"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18454,6 +18454,488 @@
         </is>
       </c>
     </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>49B6NS</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:46:40</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D536" t="n">
+        <v>401</v>
+      </c>
+      <c r="E536" t="b">
+        <v>0</v>
+      </c>
+      <c r="F536" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>36KI6F</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:46:40</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D537" t="n">
+        <v>404</v>
+      </c>
+      <c r="E537" t="b">
+        <v>0</v>
+      </c>
+      <c r="F537" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>XKGNVC</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:47:33</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D538" t="n">
+        <v>400</v>
+      </c>
+      <c r="E538" t="b">
+        <v>0</v>
+      </c>
+      <c r="F538" t="inlineStr">
+        <is>
+          <t>Model Embedder untuk 'openai' harus salah satu dari ['text-embedding-3-large', 'text-embedding-3-small'].</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>ANLMHV</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:47:40</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D539" t="n">
+        <v>200</v>
+      </c>
+      <c r="E539" t="b">
+        <v>1</v>
+      </c>
+      <c r="F539" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embedder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:1076</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>L01CA6</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:50:08</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D540" t="n">
+        <v>200</v>
+      </c>
+      <c r="E540" t="b">
+        <v>1</v>
+      </c>
+      <c r="F540" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal pmb 2025?
+###
+Answer:Salam Harmoni🙏
+Jadwal penerimaan mahasiswa baru (PMB) 2025 untuk Universitas Pendidikan Ganesha mengikuti sistem seleksi masuk perguruan tinggi negeri yang diselenggarakan oleh Panitia Seleksi Nasional Penerimaan Mahasiswa Baru (SNPMB). Sistem seleksi ini resmi dibuka pada Rabu, 11 Desember 2024. Untuk informasi lebih lanjut mengenai jadwal dan prosedur pendaftaran, Anda dapat mengunjungi situs resmi Universitas Pendidikan Ganesha.</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>D1YEPJ</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:50:37</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D541" t="n">
+        <v>200</v>
+      </c>
+      <c r="E541" t="b">
+        <v>1</v>
+      </c>
+      <c r="F541" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal penerimaan mahasiswa 2025?
+###
+Answer:Salam Harmoni🙏
+Untuk jadwal penerimaan mahasiswa baru tahun 2025 melalui Seleksi Nasional Penerimaan Mahasiswa Baru (SNPMB), informasi lengkapnya biasanya diumumkan oleh panitia SNPMB. Secara umum, jadwal penerimaan mahasiswa baru mencakup beberapa tahap, seperti pendaftaran, ujian, dan pengumuman hasil.
+Untuk informasi yang lebih akurat dan terkini, Anda dapat mengunjungi situs resmi Universitas Pendidikan Ganesha atau situs resmi SNPMB. Jika ada pertanyaan lebih lanjut, silakan tanyakan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>8HO1OY</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:51:11</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D542" t="n">
+        <v>200</v>
+      </c>
+      <c r="E542" t="b">
+        <v>1</v>
+      </c>
+      <c r="F542" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal pmb 2025?
+###
+Answer:Salam Harmoni🙏
+Jadwal penerimaan mahasiswa baru (PMB) 2025 untuk Universitas Pendidikan Ganesha mengikuti sistem seleksi masuk perguruan tinggi negeri yang diselenggarakan oleh Panitia Seleksi Nasional Penerimaan Mahasiswa Baru (SNPMB). Sistem seleksi ini resmi dibuka pada Rabu, 11 Desember 2024. Untuk informasi lebih lanjut mengenai jadwal dan prosedur pendaftaran, Anda dapat mengunjungi situs resmi Universitas Pendidikan Ganesha atau situs SNPMB.</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>PNDI2K</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:51:28</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D543" t="n">
+        <v>200</v>
+      </c>
+      <c r="E543" t="b">
+        <v>1</v>
+      </c>
+      <c r="F543" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal pmb?
+###
+Answer:Salam Harmoni🙏
+Jadwal Penerimaan Mahasiswa Baru (PMB) di Universitas Pendidikan Ganesha dibedakan menjadi 3 jalur, yaitu:
+1. Jalur Seleksi Nasional Berbasis Prestasi (SNBP)
+2. Jalur Seleksi Nasional Berbasis Tes (SNBT)
+3. Jalur Seleksi Mandiri (SMBJM)
+Untuk informasi lebih lanjut mengenai waktu spesifik dari masing-masing jalur, silakan merujuk ke sumber resmi yang tersedia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>5RJVSP</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:51:48</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D544" t="n">
+        <v>200</v>
+      </c>
+      <c r="E544" t="b">
+        <v>1</v>
+      </c>
+      <c r="F544" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal snbp 2025?
+###
+Answer:Salam Harmoni🙏
+Jadwal Seleksi Nasional Berbasis Prestasi (SNBP) 2025 adalah sebagai berikut:
+1. **Pendaftaran SNBP**: 04 – 18 Februari 2025
+2. **Pengumuman Hasil SNBP**: 18 Maret 2025
+Pastikan untuk mempersiapkan segala sesuatunya sesuai dengan jadwal yang telah ditentukan. Jika ada pertanyaan lebih lanjut, silakan tanyakan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>SN5UVP</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:52:06</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D545" t="n">
+        <v>200</v>
+      </c>
+      <c r="E545" t="b">
+        <v>1</v>
+      </c>
+      <c r="F545" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal snbp 2025?
+###
+Answer:Salam Harmoni🙏
+Jadwal Seleksi Nasional Berbasis Prestasi (SNBP) 2025 adalah sebagai berikut:
+1. **Pendaftaran SNBP**: 04 – 18 Februari 2025
+2. **Pengumuman Hasil SNBP**: 18 Maret 2025
+Jika Anda memerlukan informasi lebih lanjut, silakan tanyakan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>9OHAZ3</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:52:22</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D546" t="n">
+        <v>200</v>
+      </c>
+      <c r="E546" t="b">
+        <v>1</v>
+      </c>
+      <c r="F546" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal snbp?
+###
+Answer:Salam Harmoni🙏
+Jadwal Seleksi Nasional Berbasis Prestasi (SNBP) 2025 adalah sebagai berikut:
+1. Pengumuman Kuota Sekolah: 28 Desember 2024
+2. Masa Sanggah: 28 Desember 2024 – 17 Januari 2025
+3. Registrasi Akun SNPMB Sekolah: 06 – 31 Januari 2025
+4. Pengisian PDSS oleh Sekolah: 06 – 31 Januari 2025
+5. Registrasi Akun SNPMB Siswa: 13 Januari – 18 Februari 2025
+6. Pendaftaran SNBP: 04 – 18 Februari 2025
+7. Pengumuman Hasil SNBP: 18 Maret 2025
+8. Masa Unduh Kartu Peserta SNBP: 4 Februari – 30 April 2025
+Jika ada pertanyaan lebih lanjut, silakan tanyakan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>KN2C1P</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:52:40</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D547" t="n">
+        <v>200</v>
+      </c>
+      <c r="E547" t="b">
+        <v>1</v>
+      </c>
+      <c r="F547" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:kapan jadwal snbt?
+###
+Answer:Salam Harmoni🙏
+Jadwal Seleksi Nasional Berbasis Tes (SNBT) adalah sebagai berikut:
+1. **Pendaftaran UTBK dan SNBT**: 11 – 27 Maret 2025
+2. **Pelaksanaan UTBK**: 
+   - Gelombang 1: 23 – 30 April 2025
+   - Gelombang 2: 2 – 3 Mei 2025
+3. **Pengumuman Hasil Seleksi Jalur SNBT**: 28 Mei 2025
+Jika ada pertanyaan lebih lanjut, silakan tanyakan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>WUF4D5</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:54:05</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D548" t="n">
+        <v>200</v>
+      </c>
+      <c r="E548" t="b">
+        <v>1</v>
+      </c>
+      <c r="F548" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:rektor undiksha
+###
+Answer:Salam Harmoni🙏
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>NBJ96M</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>2024-12-26 09:54:20</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D549" t="n">
+        <v>200</v>
+      </c>
+      <c r="E549" t="b">
+        <v>1</v>
+      </c>
+      <c r="F549" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:siapa rektor undiksha?
+###
+Answer:Salam Harmoni🙏
+Rektor Universitas Pendidikan Ganesha (Undiksha) adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>